<commit_message>
the most up-to-date proforma spreadsheet
git-svn-id: https://svn.urbansim.org/src/trunk@18045 1513fa5d-83ce-422e-ae47-6967bb0fb594
</commit_message>
<xml_diff>
--- a/urbansim_parcel/proposal/proforma.xlsx
+++ b/urbansim_parcel/proposal/proforma.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="-45" windowWidth="21405" windowHeight="12660" tabRatio="680" activeTab="1"/>
+    <workbookView xWindow="-75" yWindow="-45" windowWidth="21405" windowHeight="12660" tabRatio="680" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="4" r:id="rId1"/>
@@ -2509,9 +2509,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E53" sqref="E53"/>
+      <selection pane="topRight" activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -2740,35 +2740,35 @@
       </c>
       <c r="G6" s="5">
         <f>IF(AND(G$3&gt;='Proforma Inputs'!$B$44,G59&gt;0),IF(G59&lt;'Proforma Inputs'!$B53,G59,'Proforma Inputs'!$B53),0)</f>
-        <v>250000</v>
+        <v>0</v>
       </c>
       <c r="H6" s="5">
         <f>IF(AND(H$3&gt;='Proforma Inputs'!$B$44,H59&gt;0),IF(H59&lt;'Proforma Inputs'!$B53,H59,'Proforma Inputs'!$B53),0)</f>
-        <v>250000</v>
+        <v>0</v>
       </c>
       <c r="I6" s="5">
         <f>IF(AND(I$3&gt;='Proforma Inputs'!$B$44,I59&gt;0),IF(I59&lt;'Proforma Inputs'!$B53,I59,'Proforma Inputs'!$B53),0)</f>
-        <v>250000</v>
+        <v>0</v>
       </c>
       <c r="J6" s="5">
         <f>IF(AND(J$3&gt;='Proforma Inputs'!$B$44,J59&gt;0),IF(J59&lt;'Proforma Inputs'!$B53,J59,'Proforma Inputs'!$B53),0)</f>
-        <v>250000</v>
+        <v>0</v>
       </c>
       <c r="K6" s="5">
         <f>IF(AND(K$3&gt;='Proforma Inputs'!$B$44,K59&gt;0),IF(K59&lt;'Proforma Inputs'!$B53,K59,'Proforma Inputs'!$B53),0)</f>
-        <v>250000</v>
+        <v>0</v>
       </c>
       <c r="L6" s="5">
         <f>IF(AND(L$3&gt;='Proforma Inputs'!$B$44,L59&gt;0),IF(L59&lt;'Proforma Inputs'!$B53,L59,'Proforma Inputs'!$B53),0)</f>
-        <v>250000</v>
+        <v>0</v>
       </c>
       <c r="M6" s="5">
         <f>IF(AND(M$3&gt;='Proforma Inputs'!$B$44,M59&gt;0),IF(M59&lt;'Proforma Inputs'!$B53,M59,'Proforma Inputs'!$B53),0)</f>
-        <v>250000</v>
+        <v>0</v>
       </c>
       <c r="N6" s="5">
         <f>IF(AND(N$3&gt;='Proforma Inputs'!$B$44,N59&gt;0),IF(N59&lt;'Proforma Inputs'!$B53,N59,'Proforma Inputs'!$B53),0)</f>
-        <v>250000</v>
+        <v>0</v>
       </c>
       <c r="O6" s="5">
         <f>IF(AND(O$3&gt;='Proforma Inputs'!$B$44,O59&gt;0),IF(O59&lt;'Proforma Inputs'!$B53,O59,'Proforma Inputs'!$B53),0)</f>
@@ -2914,43 +2914,43 @@
       </c>
       <c r="G7" s="5">
         <f>IF(AND(G$3&gt;='Proforma Inputs'!$B$44,G60&gt;0),IF(G60&lt;'Proforma Inputs'!$B54,G60,'Proforma Inputs'!$B54),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="H7" s="5">
         <f>IF(AND(H$3&gt;='Proforma Inputs'!$B$44,H60&gt;0),IF(H60&lt;'Proforma Inputs'!$B54,H60,'Proforma Inputs'!$B54),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="I7" s="5">
         <f>IF(AND(I$3&gt;='Proforma Inputs'!$B$44,I60&gt;0),IF(I60&lt;'Proforma Inputs'!$B54,I60,'Proforma Inputs'!$B54),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="J7" s="5">
         <f>IF(AND(J$3&gt;='Proforma Inputs'!$B$44,J60&gt;0),IF(J60&lt;'Proforma Inputs'!$B54,J60,'Proforma Inputs'!$B54),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="K7" s="5">
         <f>IF(AND(K$3&gt;='Proforma Inputs'!$B$44,K60&gt;0),IF(K60&lt;'Proforma Inputs'!$B54,K60,'Proforma Inputs'!$B54),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="L7" s="5">
         <f>IF(AND(L$3&gt;='Proforma Inputs'!$B$44,L60&gt;0),IF(L60&lt;'Proforma Inputs'!$B54,L60,'Proforma Inputs'!$B54),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="M7" s="5">
         <f>IF(AND(M$3&gt;='Proforma Inputs'!$B$44,M60&gt;0),IF(M60&lt;'Proforma Inputs'!$B54,M60,'Proforma Inputs'!$B54),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="N7" s="5">
         <f>IF(AND(N$3&gt;='Proforma Inputs'!$B$44,N60&gt;0),IF(N60&lt;'Proforma Inputs'!$B54,N60,'Proforma Inputs'!$B54),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="O7" s="5">
         <f>IF(AND(O$3&gt;='Proforma Inputs'!$B$44,O60&gt;0),IF(O60&lt;'Proforma Inputs'!$B54,O60,'Proforma Inputs'!$B54),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="P7" s="5">
         <f>IF(AND(P$3&gt;='Proforma Inputs'!$B$44,P60&gt;0),IF(P60&lt;'Proforma Inputs'!$B54,P60,'Proforma Inputs'!$B54),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="5">
         <f>IF(AND(Q$3&gt;='Proforma Inputs'!$B$44,Q60&gt;0),IF(Q60&lt;'Proforma Inputs'!$B54,Q60,'Proforma Inputs'!$B54),0)</f>
@@ -3088,51 +3088,51 @@
       </c>
       <c r="G8" s="5">
         <f>IF(AND(G$3&gt;='Proforma Inputs'!$B$44,G61&gt;0),IF(G61&lt;'Proforma Inputs'!$B55,G61,'Proforma Inputs'!$B55),0)</f>
-        <v>350000</v>
+        <v>0</v>
       </c>
       <c r="H8" s="5">
         <f>IF(AND(H$3&gt;='Proforma Inputs'!$B$44,H61&gt;0),IF(H61&lt;'Proforma Inputs'!$B55,H61,'Proforma Inputs'!$B55),0)</f>
-        <v>350000</v>
+        <v>0</v>
       </c>
       <c r="I8" s="5">
         <f>IF(AND(I$3&gt;='Proforma Inputs'!$B$44,I61&gt;0),IF(I61&lt;'Proforma Inputs'!$B55,I61,'Proforma Inputs'!$B55),0)</f>
-        <v>350000</v>
+        <v>0</v>
       </c>
       <c r="J8" s="5">
         <f>IF(AND(J$3&gt;='Proforma Inputs'!$B$44,J61&gt;0),IF(J61&lt;'Proforma Inputs'!$B55,J61,'Proforma Inputs'!$B55),0)</f>
-        <v>350000</v>
+        <v>0</v>
       </c>
       <c r="K8" s="5">
         <f>IF(AND(K$3&gt;='Proforma Inputs'!$B$44,K61&gt;0),IF(K61&lt;'Proforma Inputs'!$B55,K61,'Proforma Inputs'!$B55),0)</f>
-        <v>350000</v>
+        <v>0</v>
       </c>
       <c r="L8" s="5">
         <f>IF(AND(L$3&gt;='Proforma Inputs'!$B$44,L61&gt;0),IF(L61&lt;'Proforma Inputs'!$B55,L61,'Proforma Inputs'!$B55),0)</f>
-        <v>350000</v>
+        <v>0</v>
       </c>
       <c r="M8" s="5">
         <f>IF(AND(M$3&gt;='Proforma Inputs'!$B$44,M61&gt;0),IF(M61&lt;'Proforma Inputs'!$B55,M61,'Proforma Inputs'!$B55),0)</f>
-        <v>350000</v>
+        <v>0</v>
       </c>
       <c r="N8" s="5">
         <f>IF(AND(N$3&gt;='Proforma Inputs'!$B$44,N61&gt;0),IF(N61&lt;'Proforma Inputs'!$B55,N61,'Proforma Inputs'!$B55),0)</f>
-        <v>350000</v>
+        <v>0</v>
       </c>
       <c r="O8" s="5">
         <f>IF(AND(O$3&gt;='Proforma Inputs'!$B$44,O61&gt;0),IF(O61&lt;'Proforma Inputs'!$B55,O61,'Proforma Inputs'!$B55),0)</f>
-        <v>350000</v>
+        <v>0</v>
       </c>
       <c r="P8" s="5">
         <f>IF(AND(P$3&gt;='Proforma Inputs'!$B$44,P61&gt;0),IF(P61&lt;'Proforma Inputs'!$B55,P61,'Proforma Inputs'!$B55),0)</f>
-        <v>350000</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="5">
         <f>IF(AND(Q$3&gt;='Proforma Inputs'!$B$44,Q61&gt;0),IF(Q61&lt;'Proforma Inputs'!$B55,Q61,'Proforma Inputs'!$B55),0)</f>
-        <v>350000</v>
+        <v>0</v>
       </c>
       <c r="R8" s="5">
         <f>IF(AND(R$3&gt;='Proforma Inputs'!$B$44,R61&gt;0),IF(R61&lt;'Proforma Inputs'!$B55,R61,'Proforma Inputs'!$B55),0)</f>
-        <v>150000</v>
+        <v>0</v>
       </c>
       <c r="S8" s="5">
         <f>IF(AND(S$3&gt;='Proforma Inputs'!$B$44,S61&gt;0),IF(S61&lt;'Proforma Inputs'!$B55,S61,'Proforma Inputs'!$B55),0)</f>
@@ -3262,55 +3262,55 @@
       </c>
       <c r="G9" s="25">
         <f>IF(AND(G$3&gt;='Proforma Inputs'!$B$44,G62&gt;0),IF(G62&lt;'Proforma Inputs'!$B56,G62,'Proforma Inputs'!$B56),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="H9" s="25">
         <f>IF(AND(H$3&gt;='Proforma Inputs'!$B$44,H62&gt;0),IF(H62&lt;'Proforma Inputs'!$B56,H62,'Proforma Inputs'!$B56),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="I9" s="25">
         <f>IF(AND(I$3&gt;='Proforma Inputs'!$B$44,I62&gt;0),IF(I62&lt;'Proforma Inputs'!$B56,I62,'Proforma Inputs'!$B56),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="J9" s="25">
         <f>IF(AND(J$3&gt;='Proforma Inputs'!$B$44,J62&gt;0),IF(J62&lt;'Proforma Inputs'!$B56,J62,'Proforma Inputs'!$B56),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="K9" s="25">
         <f>IF(AND(K$3&gt;='Proforma Inputs'!$B$44,K62&gt;0),IF(K62&lt;'Proforma Inputs'!$B56,K62,'Proforma Inputs'!$B56),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="L9" s="25">
         <f>IF(AND(L$3&gt;='Proforma Inputs'!$B$44,L62&gt;0),IF(L62&lt;'Proforma Inputs'!$B56,L62,'Proforma Inputs'!$B56),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="M9" s="25">
         <f>IF(AND(M$3&gt;='Proforma Inputs'!$B$44,M62&gt;0),IF(M62&lt;'Proforma Inputs'!$B56,M62,'Proforma Inputs'!$B56),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="N9" s="25">
         <f>IF(AND(N$3&gt;='Proforma Inputs'!$B$44,N62&gt;0),IF(N62&lt;'Proforma Inputs'!$B56,N62,'Proforma Inputs'!$B56),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="O9" s="25">
         <f>IF(AND(O$3&gt;='Proforma Inputs'!$B$44,O62&gt;0),IF(O62&lt;'Proforma Inputs'!$B56,O62,'Proforma Inputs'!$B56),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="P9" s="25">
         <f>IF(AND(P$3&gt;='Proforma Inputs'!$B$44,P62&gt;0),IF(P62&lt;'Proforma Inputs'!$B56,P62,'Proforma Inputs'!$B56),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="25">
         <f>IF(AND(Q$3&gt;='Proforma Inputs'!$B$44,Q62&gt;0),IF(Q62&lt;'Proforma Inputs'!$B56,Q62,'Proforma Inputs'!$B56),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="R9" s="25">
         <f>IF(AND(R$3&gt;='Proforma Inputs'!$B$44,R62&gt;0),IF(R62&lt;'Proforma Inputs'!$B56,R62,'Proforma Inputs'!$B56),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="S9" s="25">
         <f>IF(AND(S$3&gt;='Proforma Inputs'!$B$44,S62&gt;0),IF(S62&lt;'Proforma Inputs'!$B56,S62,'Proforma Inputs'!$B56),0)</f>
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="T9" s="25">
         <f>IF(AND(T$3&gt;='Proforma Inputs'!$B$44,T62&gt;0),IF(T62&lt;'Proforma Inputs'!$B56,T62,'Proforma Inputs'!$B56),0)</f>
@@ -4195,59 +4195,59 @@
       </c>
       <c r="G16" s="22">
         <f>IF(AND(G$3&gt;='Proforma Inputs'!$B$44,G$89=0),IF(F16&lt;'Proforma Inputs'!$B74,F16+'Proforma Inputs'!$B74/'Proforma Inputs'!$B79,F16),0)</f>
-        <v>12500</v>
+        <v>0</v>
       </c>
       <c r="H16" s="22">
         <f>IF(AND(H$3&gt;='Proforma Inputs'!$B$44,H$89=0),IF(G16&lt;'Proforma Inputs'!$B74,G16+'Proforma Inputs'!$B74/'Proforma Inputs'!$B79,G16),0)</f>
-        <v>25000</v>
+        <v>0</v>
       </c>
       <c r="I16" s="22">
         <f>IF(AND(I$3&gt;='Proforma Inputs'!$B$44,I$89=0),IF(H16&lt;'Proforma Inputs'!$B74,H16+'Proforma Inputs'!$B74/'Proforma Inputs'!$B79,H16),0)</f>
-        <v>37500</v>
+        <v>0</v>
       </c>
       <c r="J16" s="22">
         <f>IF(AND(J$3&gt;='Proforma Inputs'!$B$44,J$89=0),IF(I16&lt;'Proforma Inputs'!$B74,I16+'Proforma Inputs'!$B74/'Proforma Inputs'!$B79,I16),0)</f>
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="K16" s="22">
         <f>IF(AND(K$3&gt;='Proforma Inputs'!$B$44,K$89=0),IF(J16&lt;'Proforma Inputs'!$B74,J16+'Proforma Inputs'!$B74/'Proforma Inputs'!$B79,J16),0)</f>
-        <v>62500</v>
+        <v>0</v>
       </c>
       <c r="L16" s="22">
         <f>IF(AND(L$3&gt;='Proforma Inputs'!$B$44,L$89=0),IF(K16&lt;'Proforma Inputs'!$B74,K16+'Proforma Inputs'!$B74/'Proforma Inputs'!$B79,K16),0)</f>
-        <v>75000</v>
+        <v>0</v>
       </c>
       <c r="M16" s="22">
         <f>IF(AND(M$3&gt;='Proforma Inputs'!$B$44,M$89=0),IF(L16&lt;'Proforma Inputs'!$B74,L16+'Proforma Inputs'!$B74/'Proforma Inputs'!$B79,L16),0)</f>
-        <v>87500</v>
+        <v>0</v>
       </c>
       <c r="N16" s="22">
         <f>IF(AND(N$3&gt;='Proforma Inputs'!$B$44,N$89=0),IF(M16&lt;'Proforma Inputs'!$B74,M16+'Proforma Inputs'!$B74/'Proforma Inputs'!$B79,M16),0)</f>
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="O16" s="22">
         <f>IF(AND(O$3&gt;='Proforma Inputs'!$B$44,O$89=0),IF(N16&lt;'Proforma Inputs'!$B74,N16+'Proforma Inputs'!$B74/'Proforma Inputs'!$B79,N16),0)</f>
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="P16" s="22">
         <f>IF(AND(P$3&gt;='Proforma Inputs'!$B$44,P$89=0),IF(O16&lt;'Proforma Inputs'!$B74,O16+'Proforma Inputs'!$B74/'Proforma Inputs'!$B79,O16),0)</f>
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="22">
         <f>IF(AND(Q$3&gt;='Proforma Inputs'!$B$44,Q$89=0),IF(P16&lt;'Proforma Inputs'!$B74,P16+'Proforma Inputs'!$B74/'Proforma Inputs'!$B79,P16),0)</f>
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="R16" s="22">
         <f>IF(AND(R$3&gt;='Proforma Inputs'!$B$44,R$89=0),IF(Q16&lt;'Proforma Inputs'!$B74,Q16+'Proforma Inputs'!$B74/'Proforma Inputs'!$B79,Q16),0)</f>
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="S16" s="22">
         <f>IF(AND(S$3&gt;='Proforma Inputs'!$B$44,S$89=0),IF(R16&lt;'Proforma Inputs'!$B74,R16+'Proforma Inputs'!$B74/'Proforma Inputs'!$B79,R16),0)</f>
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="T16" s="22">
         <f>IF(AND(T$3&gt;='Proforma Inputs'!$B$44,T$89=0),IF(S16&lt;'Proforma Inputs'!$B74,S16+'Proforma Inputs'!$B74/'Proforma Inputs'!$B79,S16),0)</f>
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="U16" s="22">
         <f>IF(AND(U$3&gt;='Proforma Inputs'!$B$44,U$89=0),IF(T16&lt;'Proforma Inputs'!$B74,T16+'Proforma Inputs'!$B74/'Proforma Inputs'!$B79,T16),0)</f>
@@ -4369,59 +4369,59 @@
       </c>
       <c r="G17" s="22">
         <f>IF(AND(G$3&gt;='Proforma Inputs'!$B$44,G$89=0),IF(F17&lt;'Proforma Inputs'!$B75,F17+'Proforma Inputs'!$B75/'Proforma Inputs'!$B80,F17),0)</f>
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="H17" s="22">
         <f>IF(AND(H$3&gt;='Proforma Inputs'!$B$44,H$89=0),IF(G17&lt;'Proforma Inputs'!$B75,G17+'Proforma Inputs'!$B75/'Proforma Inputs'!$B80,G17),0)</f>
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="I17" s="22">
         <f>IF(AND(I$3&gt;='Proforma Inputs'!$B$44,I$89=0),IF(H17&lt;'Proforma Inputs'!$B75,H17+'Proforma Inputs'!$B75/'Proforma Inputs'!$B80,H17),0)</f>
-        <v>150000</v>
+        <v>0</v>
       </c>
       <c r="J17" s="22">
         <f>IF(AND(J$3&gt;='Proforma Inputs'!$B$44,J$89=0),IF(I17&lt;'Proforma Inputs'!$B75,I17+'Proforma Inputs'!$B75/'Proforma Inputs'!$B80,I17),0)</f>
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="K17" s="22">
         <f>IF(AND(K$3&gt;='Proforma Inputs'!$B$44,K$89=0),IF(J17&lt;'Proforma Inputs'!$B75,J17+'Proforma Inputs'!$B75/'Proforma Inputs'!$B80,J17),0)</f>
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="L17" s="22">
         <f>IF(AND(L$3&gt;='Proforma Inputs'!$B$44,L$89=0),IF(K17&lt;'Proforma Inputs'!$B75,K17+'Proforma Inputs'!$B75/'Proforma Inputs'!$B80,K17),0)</f>
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="M17" s="22">
         <f>IF(AND(M$3&gt;='Proforma Inputs'!$B$44,M$89=0),IF(L17&lt;'Proforma Inputs'!$B75,L17+'Proforma Inputs'!$B75/'Proforma Inputs'!$B80,L17),0)</f>
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="N17" s="22">
         <f>IF(AND(N$3&gt;='Proforma Inputs'!$B$44,N$89=0),IF(M17&lt;'Proforma Inputs'!$B75,M17+'Proforma Inputs'!$B75/'Proforma Inputs'!$B80,M17),0)</f>
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="O17" s="22">
         <f>IF(AND(O$3&gt;='Proforma Inputs'!$B$44,O$89=0),IF(N17&lt;'Proforma Inputs'!$B75,N17+'Proforma Inputs'!$B75/'Proforma Inputs'!$B80,N17),0)</f>
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="P17" s="22">
         <f>IF(AND(P$3&gt;='Proforma Inputs'!$B$44,P$89=0),IF(O17&lt;'Proforma Inputs'!$B75,O17+'Proforma Inputs'!$B75/'Proforma Inputs'!$B80,O17),0)</f>
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="22">
         <f>IF(AND(Q$3&gt;='Proforma Inputs'!$B$44,Q$89=0),IF(P17&lt;'Proforma Inputs'!$B75,P17+'Proforma Inputs'!$B75/'Proforma Inputs'!$B80,P17),0)</f>
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="R17" s="22">
         <f>IF(AND(R$3&gt;='Proforma Inputs'!$B$44,R$89=0),IF(Q17&lt;'Proforma Inputs'!$B75,Q17+'Proforma Inputs'!$B75/'Proforma Inputs'!$B80,Q17),0)</f>
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="S17" s="22">
         <f>IF(AND(S$3&gt;='Proforma Inputs'!$B$44,S$89=0),IF(R17&lt;'Proforma Inputs'!$B75,R17+'Proforma Inputs'!$B75/'Proforma Inputs'!$B80,R17),0)</f>
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="T17" s="22">
         <f>IF(AND(T$3&gt;='Proforma Inputs'!$B$44,T$89=0),IF(S17&lt;'Proforma Inputs'!$B75,S17+'Proforma Inputs'!$B75/'Proforma Inputs'!$B80,S17),0)</f>
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="U17" s="22">
         <f>IF(AND(U$3&gt;='Proforma Inputs'!$B$44,U$89=0),IF(T17&lt;'Proforma Inputs'!$B75,T17+'Proforma Inputs'!$B75/'Proforma Inputs'!$B80,T17),0)</f>
@@ -4543,59 +4543,59 @@
       </c>
       <c r="G18" s="22">
         <f>IF(AND(G$3&gt;='Proforma Inputs'!$B$44,G$89=0),IF(F18&lt;'Proforma Inputs'!$B76,F18+'Proforma Inputs'!$B76/'Proforma Inputs'!$B81,F18),0)</f>
-        <v>75000</v>
+        <v>0</v>
       </c>
       <c r="H18" s="22">
         <f>IF(AND(H$3&gt;='Proforma Inputs'!$B$44,H$89=0),IF(G18&lt;'Proforma Inputs'!$B76,G18+'Proforma Inputs'!$B76/'Proforma Inputs'!$B81,G18),0)</f>
-        <v>150000</v>
+        <v>0</v>
       </c>
       <c r="I18" s="22">
         <f>IF(AND(I$3&gt;='Proforma Inputs'!$B$44,I$89=0),IF(H18&lt;'Proforma Inputs'!$B76,H18+'Proforma Inputs'!$B76/'Proforma Inputs'!$B81,H18),0)</f>
-        <v>225000</v>
+        <v>0</v>
       </c>
       <c r="J18" s="22">
         <f>IF(AND(J$3&gt;='Proforma Inputs'!$B$44,J$89=0),IF(I18&lt;'Proforma Inputs'!$B76,I18+'Proforma Inputs'!$B76/'Proforma Inputs'!$B81,I18),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="K18" s="22">
         <f>IF(AND(K$3&gt;='Proforma Inputs'!$B$44,K$89=0),IF(J18&lt;'Proforma Inputs'!$B76,J18+'Proforma Inputs'!$B76/'Proforma Inputs'!$B81,J18),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="L18" s="22">
         <f>IF(AND(L$3&gt;='Proforma Inputs'!$B$44,L$89=0),IF(K18&lt;'Proforma Inputs'!$B76,K18+'Proforma Inputs'!$B76/'Proforma Inputs'!$B81,K18),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="M18" s="22">
         <f>IF(AND(M$3&gt;='Proforma Inputs'!$B$44,M$89=0),IF(L18&lt;'Proforma Inputs'!$B76,L18+'Proforma Inputs'!$B76/'Proforma Inputs'!$B81,L18),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="N18" s="22">
         <f>IF(AND(N$3&gt;='Proforma Inputs'!$B$44,N$89=0),IF(M18&lt;'Proforma Inputs'!$B76,M18+'Proforma Inputs'!$B76/'Proforma Inputs'!$B81,M18),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="O18" s="22">
         <f>IF(AND(O$3&gt;='Proforma Inputs'!$B$44,O$89=0),IF(N18&lt;'Proforma Inputs'!$B76,N18+'Proforma Inputs'!$B76/'Proforma Inputs'!$B81,N18),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="P18" s="22">
         <f>IF(AND(P$3&gt;='Proforma Inputs'!$B$44,P$89=0),IF(O18&lt;'Proforma Inputs'!$B76,O18+'Proforma Inputs'!$B76/'Proforma Inputs'!$B81,O18),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="22">
         <f>IF(AND(Q$3&gt;='Proforma Inputs'!$B$44,Q$89=0),IF(P18&lt;'Proforma Inputs'!$B76,P18+'Proforma Inputs'!$B76/'Proforma Inputs'!$B81,P18),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="R18" s="22">
         <f>IF(AND(R$3&gt;='Proforma Inputs'!$B$44,R$89=0),IF(Q18&lt;'Proforma Inputs'!$B76,Q18+'Proforma Inputs'!$B76/'Proforma Inputs'!$B81,Q18),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="S18" s="22">
         <f>IF(AND(S$3&gt;='Proforma Inputs'!$B$44,S$89=0),IF(R18&lt;'Proforma Inputs'!$B76,R18+'Proforma Inputs'!$B76/'Proforma Inputs'!$B81,R18),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="T18" s="22">
         <f>IF(AND(T$3&gt;='Proforma Inputs'!$B$44,T$89=0),IF(S18&lt;'Proforma Inputs'!$B76,S18+'Proforma Inputs'!$B76/'Proforma Inputs'!$B81,S18),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="U18" s="22">
         <f>IF(AND(U$3&gt;='Proforma Inputs'!$B$44,U$89=0),IF(T18&lt;'Proforma Inputs'!$B76,T18+'Proforma Inputs'!$B76/'Proforma Inputs'!$B81,T18),0)</f>
@@ -4717,59 +4717,59 @@
       </c>
       <c r="G19" s="22">
         <f>IF(AND(G$3&gt;='Proforma Inputs'!$B$44,G$89=0),IF(F19&lt;'Proforma Inputs'!$B77,F19+'Proforma Inputs'!$B77/'Proforma Inputs'!$B82,F19),0)</f>
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="H19" s="22">
         <f>IF(AND(H$3&gt;='Proforma Inputs'!$B$44,H$89=0),IF(G19&lt;'Proforma Inputs'!$B77,G19+'Proforma Inputs'!$B77/'Proforma Inputs'!$B82,G19),0)</f>
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="I19" s="22">
         <f>IF(AND(I$3&gt;='Proforma Inputs'!$B$44,I$89=0),IF(H19&lt;'Proforma Inputs'!$B77,H19+'Proforma Inputs'!$B77/'Proforma Inputs'!$B82,H19),0)</f>
-        <v>150000</v>
+        <v>0</v>
       </c>
       <c r="J19" s="22">
         <f>IF(AND(J$3&gt;='Proforma Inputs'!$B$44,J$89=0),IF(I19&lt;'Proforma Inputs'!$B77,I19+'Proforma Inputs'!$B77/'Proforma Inputs'!$B82,I19),0)</f>
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="K19" s="22">
         <f>IF(AND(K$3&gt;='Proforma Inputs'!$B$44,K$89=0),IF(J19&lt;'Proforma Inputs'!$B77,J19+'Proforma Inputs'!$B77/'Proforma Inputs'!$B82,J19),0)</f>
-        <v>250000</v>
+        <v>0</v>
       </c>
       <c r="L19" s="22">
         <f>IF(AND(L$3&gt;='Proforma Inputs'!$B$44,L$89=0),IF(K19&lt;'Proforma Inputs'!$B77,K19+'Proforma Inputs'!$B77/'Proforma Inputs'!$B82,K19),0)</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="M19" s="22">
         <f>IF(AND(M$3&gt;='Proforma Inputs'!$B$44,M$89=0),IF(L19&lt;'Proforma Inputs'!$B77,L19+'Proforma Inputs'!$B77/'Proforma Inputs'!$B82,L19),0)</f>
-        <v>350000</v>
+        <v>0</v>
       </c>
       <c r="N19" s="22">
         <f>IF(AND(N$3&gt;='Proforma Inputs'!$B$44,N$89=0),IF(M19&lt;'Proforma Inputs'!$B77,M19+'Proforma Inputs'!$B77/'Proforma Inputs'!$B82,M19),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="O19" s="22">
         <f>IF(AND(O$3&gt;='Proforma Inputs'!$B$44,O$89=0),IF(N19&lt;'Proforma Inputs'!$B77,N19+'Proforma Inputs'!$B77/'Proforma Inputs'!$B82,N19),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="P19" s="22">
         <f>IF(AND(P$3&gt;='Proforma Inputs'!$B$44,P$89=0),IF(O19&lt;'Proforma Inputs'!$B77,O19+'Proforma Inputs'!$B77/'Proforma Inputs'!$B82,O19),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="22">
         <f>IF(AND(Q$3&gt;='Proforma Inputs'!$B$44,Q$89=0),IF(P19&lt;'Proforma Inputs'!$B77,P19+'Proforma Inputs'!$B77/'Proforma Inputs'!$B82,P19),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="R19" s="22">
         <f>IF(AND(R$3&gt;='Proforma Inputs'!$B$44,R$89=0),IF(Q19&lt;'Proforma Inputs'!$B77,Q19+'Proforma Inputs'!$B77/'Proforma Inputs'!$B82,Q19),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="S19" s="22">
         <f>IF(AND(S$3&gt;='Proforma Inputs'!$B$44,S$89=0),IF(R19&lt;'Proforma Inputs'!$B77,R19+'Proforma Inputs'!$B77/'Proforma Inputs'!$B82,R19),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="T19" s="22">
         <f>IF(AND(T$3&gt;='Proforma Inputs'!$B$44,T$89=0),IF(S19&lt;'Proforma Inputs'!$B77,S19+'Proforma Inputs'!$B77/'Proforma Inputs'!$B82,S19),0)</f>
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="U19" s="22">
         <f>IF(AND(U$3&gt;='Proforma Inputs'!$B$44,U$89=0),IF(T19&lt;'Proforma Inputs'!$B77,T19+'Proforma Inputs'!$B77/'Proforma Inputs'!$B82,T19),0)</f>
@@ -4896,59 +4896,59 @@
       </c>
       <c r="G21" s="22">
         <f>IF(AND(G$3&gt;='Proforma Inputs'!$B$44,G$89=0),IF(F21&lt;'Proforma Inputs'!$B92,F21+'Proforma Inputs'!$B92/'Proforma Inputs'!$B100,F21),0)</f>
-        <v>500000</v>
+        <v>0</v>
       </c>
       <c r="H21" s="22">
         <f>IF(AND(H$3&gt;='Proforma Inputs'!$B$44,H$89=0),IF(G21&lt;'Proforma Inputs'!$B92,G21+'Proforma Inputs'!$B92/'Proforma Inputs'!$B100,G21),0)</f>
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="I21" s="22">
         <f>IF(AND(I$3&gt;='Proforma Inputs'!$B$44,I$89=0),IF(H21&lt;'Proforma Inputs'!$B92,H21+'Proforma Inputs'!$B92/'Proforma Inputs'!$B100,H21),0)</f>
-        <v>1500000</v>
+        <v>0</v>
       </c>
       <c r="J21" s="22">
         <f>IF(AND(J$3&gt;='Proforma Inputs'!$B$44,J$89=0),IF(I21&lt;'Proforma Inputs'!$B92,I21+'Proforma Inputs'!$B92/'Proforma Inputs'!$B100,I21),0)</f>
-        <v>2000000</v>
+        <v>0</v>
       </c>
       <c r="K21" s="22">
         <f>IF(AND(K$3&gt;='Proforma Inputs'!$B$44,K$89=0),IF(J21&lt;'Proforma Inputs'!$B92,J21+'Proforma Inputs'!$B92/'Proforma Inputs'!$B100,J21),0)</f>
-        <v>2500000</v>
+        <v>0</v>
       </c>
       <c r="L21" s="22">
         <f>IF(AND(L$3&gt;='Proforma Inputs'!$B$44,L$89=0),IF(K21&lt;'Proforma Inputs'!$B92,K21+'Proforma Inputs'!$B92/'Proforma Inputs'!$B100,K21),0)</f>
-        <v>3000000</v>
+        <v>0</v>
       </c>
       <c r="M21" s="22">
         <f>IF(AND(M$3&gt;='Proforma Inputs'!$B$44,M$89=0),IF(L21&lt;'Proforma Inputs'!$B92,L21+'Proforma Inputs'!$B92/'Proforma Inputs'!$B100,L21),0)</f>
-        <v>3500000</v>
+        <v>0</v>
       </c>
       <c r="N21" s="22">
         <f>IF(AND(N$3&gt;='Proforma Inputs'!$B$44,N$89=0),IF(M21&lt;'Proforma Inputs'!$B92,M21+'Proforma Inputs'!$B92/'Proforma Inputs'!$B100,M21),0)</f>
-        <v>4000000</v>
+        <v>0</v>
       </c>
       <c r="O21" s="22">
         <f>IF(AND(O$3&gt;='Proforma Inputs'!$B$44,O$89=0),IF(N21&lt;'Proforma Inputs'!$B92,N21+'Proforma Inputs'!$B92/'Proforma Inputs'!$B100,N21),0)</f>
-        <v>4000000</v>
+        <v>0</v>
       </c>
       <c r="P21" s="22">
         <f>IF(AND(P$3&gt;='Proforma Inputs'!$B$44,P$89=0),IF(O21&lt;'Proforma Inputs'!$B92,O21+'Proforma Inputs'!$B92/'Proforma Inputs'!$B100,O21),0)</f>
-        <v>4000000</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="22">
         <f>IF(AND(Q$3&gt;='Proforma Inputs'!$B$44,Q$89=0),IF(P21&lt;'Proforma Inputs'!$B92,P21+'Proforma Inputs'!$B92/'Proforma Inputs'!$B100,P21),0)</f>
-        <v>4000000</v>
+        <v>0</v>
       </c>
       <c r="R21" s="22">
         <f>IF(AND(R$3&gt;='Proforma Inputs'!$B$44,R$89=0),IF(Q21&lt;'Proforma Inputs'!$B92,Q21+'Proforma Inputs'!$B92/'Proforma Inputs'!$B100,Q21),0)</f>
-        <v>4000000</v>
+        <v>0</v>
       </c>
       <c r="S21" s="22">
         <f>IF(AND(S$3&gt;='Proforma Inputs'!$B$44,S$89=0),IF(R21&lt;'Proforma Inputs'!$B92,R21+'Proforma Inputs'!$B92/'Proforma Inputs'!$B100,R21),0)</f>
-        <v>4000000</v>
+        <v>0</v>
       </c>
       <c r="T21" s="22">
         <f>IF(AND(T$3&gt;='Proforma Inputs'!$B$44,T$89=0),IF(S21&lt;'Proforma Inputs'!$B92,S21+'Proforma Inputs'!$B92/'Proforma Inputs'!$B100,S21),0)</f>
-        <v>4000000</v>
+        <v>0</v>
       </c>
       <c r="U21" s="22">
         <f>IF(AND(U$3&gt;='Proforma Inputs'!$B$44,U$89=0),IF(T21&lt;'Proforma Inputs'!$B92,T21+'Proforma Inputs'!$B92/'Proforma Inputs'!$B100,T21),0)</f>
@@ -6114,7 +6114,7 @@
       </c>
       <c r="G28" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-121428.57142857142</v>
       </c>
       <c r="H28" s="22">
         <f t="shared" si="0"/>
@@ -6166,7 +6166,7 @@
       </c>
       <c r="T28" s="22">
         <f t="shared" si="0"/>
-        <v>53124999.999999993</v>
+        <v>0</v>
       </c>
       <c r="U28" s="22">
         <f t="shared" si="0"/>
@@ -6462,7 +6462,7 @@
       </c>
       <c r="G30" s="17">
         <f t="shared" si="1"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="H30" s="17">
         <f t="shared" si="1"/>
@@ -6636,59 +6636,59 @@
       </c>
       <c r="G31" s="6">
         <f t="shared" si="2"/>
-        <v>3488431.5361752608</v>
+        <v>-121428.57142857142</v>
       </c>
       <c r="H31" s="6">
         <f t="shared" si="2"/>
-        <v>2675000</v>
+        <v>0</v>
       </c>
       <c r="I31" s="6">
         <f t="shared" si="2"/>
-        <v>3362500</v>
+        <v>0</v>
       </c>
       <c r="J31" s="6">
         <f t="shared" si="2"/>
-        <v>4050000</v>
+        <v>0</v>
       </c>
       <c r="K31" s="6">
         <f t="shared" si="2"/>
-        <v>4612500</v>
+        <v>0</v>
       </c>
       <c r="L31" s="6">
         <f t="shared" si="2"/>
-        <v>5175000</v>
+        <v>0</v>
       </c>
       <c r="M31" s="6">
         <f t="shared" si="2"/>
-        <v>5737500</v>
+        <v>0</v>
       </c>
       <c r="N31" s="6">
         <f t="shared" si="2"/>
-        <v>6300000</v>
+        <v>0</v>
       </c>
       <c r="O31" s="6">
         <f t="shared" si="2"/>
-        <v>6050000</v>
+        <v>0</v>
       </c>
       <c r="P31" s="6">
         <f t="shared" si="2"/>
-        <v>6050000</v>
+        <v>0</v>
       </c>
       <c r="Q31" s="6">
         <f t="shared" si="2"/>
-        <v>5750000</v>
+        <v>0</v>
       </c>
       <c r="R31" s="6">
         <f t="shared" si="2"/>
-        <v>5550000</v>
+        <v>0</v>
       </c>
       <c r="S31" s="6">
         <f t="shared" si="2"/>
-        <v>5200000</v>
+        <v>0</v>
       </c>
       <c r="T31" s="6">
         <f t="shared" si="2"/>
-        <v>58124999.999999993</v>
+        <v>0</v>
       </c>
       <c r="U31" s="6">
         <f t="shared" si="2"/>
@@ -6964,59 +6964,59 @@
       </c>
       <c r="G35" s="5">
         <f>IF(AND(G89=0,G3&gt;='Proforma Inputs'!$B$44),-('Proforma Inputs'!$B$41+'Proforma Inputs'!$B$40)*('Proforma Inputs'!$B$71/'Proforma Inputs'!$B$72)*'Proforma Inputs'!$B$17,0)</f>
-        <v>-350000</v>
+        <v>-1000</v>
       </c>
       <c r="H35" s="5">
         <f>IF(AND(H89=0,H3&gt;='Proforma Inputs'!$B$44),-('Proforma Inputs'!$B$41+'Proforma Inputs'!$B$40)*('Proforma Inputs'!$B$71/'Proforma Inputs'!$B$72)*'Proforma Inputs'!$B$17,0)</f>
-        <v>-350000</v>
+        <v>0</v>
       </c>
       <c r="I35" s="5">
         <f>IF(AND(I89=0,I3&gt;='Proforma Inputs'!$B$44),-('Proforma Inputs'!$B$41+'Proforma Inputs'!$B$40)*('Proforma Inputs'!$B$71/'Proforma Inputs'!$B$72)*'Proforma Inputs'!$B$17,0)</f>
-        <v>-350000</v>
+        <v>0</v>
       </c>
       <c r="J35" s="5">
         <f>IF(AND(J89=0,J3&gt;='Proforma Inputs'!$B$44),-('Proforma Inputs'!$B$41+'Proforma Inputs'!$B$40)*('Proforma Inputs'!$B$71/'Proforma Inputs'!$B$72)*'Proforma Inputs'!$B$17,0)</f>
-        <v>-350000</v>
+        <v>0</v>
       </c>
       <c r="K35" s="5">
         <f>IF(AND(K89=0,K3&gt;='Proforma Inputs'!$B$44),-('Proforma Inputs'!$B$41+'Proforma Inputs'!$B$40)*('Proforma Inputs'!$B$71/'Proforma Inputs'!$B$72)*'Proforma Inputs'!$B$17,0)</f>
-        <v>-350000</v>
+        <v>0</v>
       </c>
       <c r="L35" s="5">
         <f>IF(AND(L89=0,L3&gt;='Proforma Inputs'!$B$44),-('Proforma Inputs'!$B$41+'Proforma Inputs'!$B$40)*('Proforma Inputs'!$B$71/'Proforma Inputs'!$B$72)*'Proforma Inputs'!$B$17,0)</f>
-        <v>-350000</v>
+        <v>0</v>
       </c>
       <c r="M35" s="5">
         <f>IF(AND(M89=0,M3&gt;='Proforma Inputs'!$B$44),-('Proforma Inputs'!$B$41+'Proforma Inputs'!$B$40)*('Proforma Inputs'!$B$71/'Proforma Inputs'!$B$72)*'Proforma Inputs'!$B$17,0)</f>
-        <v>-350000</v>
+        <v>0</v>
       </c>
       <c r="N35" s="5">
         <f>IF(AND(N89=0,N3&gt;='Proforma Inputs'!$B$44),-('Proforma Inputs'!$B$41+'Proforma Inputs'!$B$40)*('Proforma Inputs'!$B$71/'Proforma Inputs'!$B$72)*'Proforma Inputs'!$B$17,0)</f>
-        <v>-350000</v>
+        <v>0</v>
       </c>
       <c r="O35" s="5">
         <f>IF(AND(O89=0,O3&gt;='Proforma Inputs'!$B$44),-('Proforma Inputs'!$B$41+'Proforma Inputs'!$B$40)*('Proforma Inputs'!$B$71/'Proforma Inputs'!$B$72)*'Proforma Inputs'!$B$17,0)</f>
-        <v>-350000</v>
+        <v>0</v>
       </c>
       <c r="P35" s="5">
         <f>IF(AND(P89=0,P3&gt;='Proforma Inputs'!$B$44),-('Proforma Inputs'!$B$41+'Proforma Inputs'!$B$40)*('Proforma Inputs'!$B$71/'Proforma Inputs'!$B$72)*'Proforma Inputs'!$B$17,0)</f>
-        <v>-350000</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="5">
         <f>IF(AND(Q89=0,Q3&gt;='Proforma Inputs'!$B$44),-('Proforma Inputs'!$B$41+'Proforma Inputs'!$B$40)*('Proforma Inputs'!$B$71/'Proforma Inputs'!$B$72)*'Proforma Inputs'!$B$17,0)</f>
-        <v>-350000</v>
+        <v>0</v>
       </c>
       <c r="R35" s="5">
         <f>IF(AND(R89=0,R3&gt;='Proforma Inputs'!$B$44),-('Proforma Inputs'!$B$41+'Proforma Inputs'!$B$40)*('Proforma Inputs'!$B$71/'Proforma Inputs'!$B$72)*'Proforma Inputs'!$B$17,0)</f>
-        <v>-350000</v>
+        <v>0</v>
       </c>
       <c r="S35" s="5">
         <f>IF(AND(S89=0,S3&gt;='Proforma Inputs'!$B$44),-('Proforma Inputs'!$B$41+'Proforma Inputs'!$B$40)*('Proforma Inputs'!$B$71/'Proforma Inputs'!$B$72)*'Proforma Inputs'!$B$17,0)</f>
-        <v>-350000</v>
+        <v>0</v>
       </c>
       <c r="T35" s="5">
         <f>IF(AND(T89=0,T3&gt;='Proforma Inputs'!$B$44),-('Proforma Inputs'!$B$41+'Proforma Inputs'!$B$40)*('Proforma Inputs'!$B$71/'Proforma Inputs'!$B$72)*'Proforma Inputs'!$B$17,0)</f>
-        <v>-350000</v>
+        <v>0</v>
       </c>
       <c r="U35" s="5">
         <f>IF(AND(U89=0,U3&gt;='Proforma Inputs'!$B$44),-('Proforma Inputs'!$B$41+'Proforma Inputs'!$B$40)*('Proforma Inputs'!$B$71/'Proforma Inputs'!$B$72)*'Proforma Inputs'!$B$17,0)</f>
@@ -7138,59 +7138,59 @@
       </c>
       <c r="G36" s="5">
         <f>IF(AND(G89=0,G3&gt;='Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$18*'Proforma Inputs'!$B$71,0)</f>
-        <v>-75000</v>
+        <v>-7500</v>
       </c>
       <c r="H36" s="5">
         <f>IF(AND(H89=0,H3&gt;='Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$18*'Proforma Inputs'!$B$71,0)</f>
-        <v>-75000</v>
+        <v>0</v>
       </c>
       <c r="I36" s="5">
         <f>IF(AND(I89=0,I3&gt;='Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$18*'Proforma Inputs'!$B$71,0)</f>
-        <v>-75000</v>
+        <v>0</v>
       </c>
       <c r="J36" s="5">
         <f>IF(AND(J89=0,J3&gt;='Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$18*'Proforma Inputs'!$B$71,0)</f>
-        <v>-75000</v>
+        <v>0</v>
       </c>
       <c r="K36" s="5">
         <f>IF(AND(K89=0,K3&gt;='Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$18*'Proforma Inputs'!$B$71,0)</f>
-        <v>-75000</v>
+        <v>0</v>
       </c>
       <c r="L36" s="5">
         <f>IF(AND(L89=0,L3&gt;='Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$18*'Proforma Inputs'!$B$71,0)</f>
-        <v>-75000</v>
+        <v>0</v>
       </c>
       <c r="M36" s="5">
         <f>IF(AND(M89=0,M3&gt;='Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$18*'Proforma Inputs'!$B$71,0)</f>
-        <v>-75000</v>
+        <v>0</v>
       </c>
       <c r="N36" s="5">
         <f>IF(AND(N89=0,N3&gt;='Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$18*'Proforma Inputs'!$B$71,0)</f>
-        <v>-75000</v>
+        <v>0</v>
       </c>
       <c r="O36" s="5">
         <f>IF(AND(O89=0,O3&gt;='Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$18*'Proforma Inputs'!$B$71,0)</f>
-        <v>-75000</v>
+        <v>0</v>
       </c>
       <c r="P36" s="5">
         <f>IF(AND(P89=0,P3&gt;='Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$18*'Proforma Inputs'!$B$71,0)</f>
-        <v>-75000</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="5">
         <f>IF(AND(Q89=0,Q3&gt;='Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$18*'Proforma Inputs'!$B$71,0)</f>
-        <v>-75000</v>
+        <v>0</v>
       </c>
       <c r="R36" s="5">
         <f>IF(AND(R89=0,R3&gt;='Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$18*'Proforma Inputs'!$B$71,0)</f>
-        <v>-75000</v>
+        <v>0</v>
       </c>
       <c r="S36" s="5">
         <f>IF(AND(S89=0,S3&gt;='Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$18*'Proforma Inputs'!$B$71,0)</f>
-        <v>-75000</v>
+        <v>0</v>
       </c>
       <c r="T36" s="5">
         <f>IF(AND(T89=0,T3&gt;='Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$18*'Proforma Inputs'!$B$71,0)</f>
-        <v>-75000</v>
+        <v>0</v>
       </c>
       <c r="U36" s="5">
         <f>IF(AND(U89=0,U3&gt;='Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$18*'Proforma Inputs'!$B$71,0)</f>
@@ -7312,59 +7312,59 @@
       </c>
       <c r="G37" s="5">
         <f>-SUM(G16:G19)*'Proforma Inputs'!$B$19</f>
-        <v>-37500</v>
+        <v>0</v>
       </c>
       <c r="H37" s="5">
         <f>-SUM(H16:H19)*'Proforma Inputs'!$B$19</f>
-        <v>-75000</v>
+        <v>0</v>
       </c>
       <c r="I37" s="5">
         <f>-SUM(I16:I19)*'Proforma Inputs'!$B$19</f>
-        <v>-112500</v>
+        <v>0</v>
       </c>
       <c r="J37" s="5">
         <f>-SUM(J16:J19)*'Proforma Inputs'!$B$19</f>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="K37" s="5">
         <f>-SUM(K16:K19)*'Proforma Inputs'!$B$19</f>
-        <v>-162500</v>
+        <v>0</v>
       </c>
       <c r="L37" s="5">
         <f>-SUM(L16:L19)*'Proforma Inputs'!$B$19</f>
-        <v>-175000</v>
+        <v>0</v>
       </c>
       <c r="M37" s="5">
         <f>-SUM(M16:M19)*'Proforma Inputs'!$B$19</f>
-        <v>-187500</v>
+        <v>0</v>
       </c>
       <c r="N37" s="5">
         <f>-SUM(N16:N19)*'Proforma Inputs'!$B$19</f>
-        <v>-200000</v>
+        <v>0</v>
       </c>
       <c r="O37" s="5">
         <f>-SUM(O16:O19)*'Proforma Inputs'!$B$19</f>
-        <v>-200000</v>
+        <v>0</v>
       </c>
       <c r="P37" s="5">
         <f>-SUM(P16:P19)*'Proforma Inputs'!$B$19</f>
-        <v>-200000</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="5">
         <f>-SUM(Q16:Q19)*'Proforma Inputs'!$B$19</f>
-        <v>-200000</v>
+        <v>0</v>
       </c>
       <c r="R37" s="5">
         <f>-SUM(R16:R19)*'Proforma Inputs'!$B$19</f>
-        <v>-200000</v>
+        <v>0</v>
       </c>
       <c r="S37" s="5">
         <f>-SUM(S16:S19)*'Proforma Inputs'!$B$19</f>
-        <v>-200000</v>
+        <v>0</v>
       </c>
       <c r="T37" s="5">
         <f>-SUM(T16:T19)*'Proforma Inputs'!$B$19</f>
-        <v>-200000</v>
+        <v>0</v>
       </c>
       <c r="U37" s="5">
         <f>-SUM(U16:U19)*'Proforma Inputs'!$B$19</f>
@@ -7486,59 +7486,59 @@
       </c>
       <c r="G38" s="5">
         <f>-SUMPRODUCT(G21:G27,'Proforma Inputs'!$B21:$B27)</f>
-        <v>-50000</v>
+        <v>0</v>
       </c>
       <c r="H38" s="5">
         <f>-SUMPRODUCT(H21:H27,'Proforma Inputs'!$B21:$B27)</f>
-        <v>-100000</v>
+        <v>0</v>
       </c>
       <c r="I38" s="5">
         <f>-SUMPRODUCT(I21:I27,'Proforma Inputs'!$B21:$B27)</f>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="J38" s="5">
         <f>-SUMPRODUCT(J21:J27,'Proforma Inputs'!$B21:$B27)</f>
-        <v>-200000</v>
+        <v>0</v>
       </c>
       <c r="K38" s="5">
         <f>-SUMPRODUCT(K21:K27,'Proforma Inputs'!$B21:$B27)</f>
-        <v>-250000</v>
+        <v>0</v>
       </c>
       <c r="L38" s="5">
         <f>-SUMPRODUCT(L21:L27,'Proforma Inputs'!$B21:$B27)</f>
-        <v>-300000</v>
+        <v>0</v>
       </c>
       <c r="M38" s="5">
         <f>-SUMPRODUCT(M21:M27,'Proforma Inputs'!$B21:$B27)</f>
-        <v>-350000</v>
+        <v>0</v>
       </c>
       <c r="N38" s="5">
         <f>-SUMPRODUCT(N21:N27,'Proforma Inputs'!$B21:$B27)</f>
-        <v>-400000</v>
+        <v>0</v>
       </c>
       <c r="O38" s="5">
         <f>-SUMPRODUCT(O21:O27,'Proforma Inputs'!$B21:$B27)</f>
-        <v>-400000</v>
+        <v>0</v>
       </c>
       <c r="P38" s="5">
         <f>-SUMPRODUCT(P21:P27,'Proforma Inputs'!$B21:$B27)</f>
-        <v>-400000</v>
+        <v>0</v>
       </c>
       <c r="Q38" s="5">
         <f>-SUMPRODUCT(Q21:Q27,'Proforma Inputs'!$B21:$B27)</f>
-        <v>-400000</v>
+        <v>0</v>
       </c>
       <c r="R38" s="5">
         <f>-SUMPRODUCT(R21:R27,'Proforma Inputs'!$B21:$B27)</f>
-        <v>-400000</v>
+        <v>0</v>
       </c>
       <c r="S38" s="5">
         <f>-SUMPRODUCT(S21:S27,'Proforma Inputs'!$B21:$B27)</f>
-        <v>-400000</v>
+        <v>0</v>
       </c>
       <c r="T38" s="5">
         <f>-SUMPRODUCT(T21:T27,'Proforma Inputs'!$B21:$B27)</f>
-        <v>-400000</v>
+        <v>0</v>
       </c>
       <c r="U38" s="5">
         <f>-SUMPRODUCT(U21:U27,'Proforma Inputs'!$B21:$B27)</f>
@@ -7660,59 +7660,59 @@
       </c>
       <c r="G39" s="5">
         <f>-SUMPRODUCT(G16:G19,'Proforma Inputs'!$B84:$B87)</f>
-        <v>-8854.1666666666661</v>
+        <v>0</v>
       </c>
       <c r="H39" s="5">
         <f>-SUMPRODUCT(H16:H19,'Proforma Inputs'!$B84:$B87)</f>
-        <v>-17708.333333333332</v>
+        <v>0</v>
       </c>
       <c r="I39" s="5">
         <f>-SUMPRODUCT(I16:I19,'Proforma Inputs'!$B84:$B87)</f>
-        <v>-26562.5</v>
+        <v>0</v>
       </c>
       <c r="J39" s="5">
         <f>-SUMPRODUCT(J16:J19,'Proforma Inputs'!$B84:$B87)</f>
-        <v>-35416.666666666664</v>
+        <v>0</v>
       </c>
       <c r="K39" s="5">
         <f>-SUMPRODUCT(K16:K19,'Proforma Inputs'!$B84:$B87)</f>
-        <v>-40625</v>
+        <v>0</v>
       </c>
       <c r="L39" s="5">
         <f>-SUMPRODUCT(L16:L19,'Proforma Inputs'!$B84:$B87)</f>
-        <v>-45833.333333333328</v>
+        <v>0</v>
       </c>
       <c r="M39" s="5">
         <f>-SUMPRODUCT(M16:M19,'Proforma Inputs'!$B84:$B87)</f>
-        <v>-51041.666666666664</v>
+        <v>0</v>
       </c>
       <c r="N39" s="5">
         <f>-SUMPRODUCT(N16:N19,'Proforma Inputs'!$B84:$B87)</f>
-        <v>-56249.999999999993</v>
+        <v>0</v>
       </c>
       <c r="O39" s="5">
         <f>-SUMPRODUCT(O16:O19,'Proforma Inputs'!$B84:$B87)</f>
-        <v>-56249.999999999993</v>
+        <v>0</v>
       </c>
       <c r="P39" s="5">
         <f>-SUMPRODUCT(P16:P19,'Proforma Inputs'!$B84:$B87)</f>
-        <v>-56249.999999999993</v>
+        <v>0</v>
       </c>
       <c r="Q39" s="5">
         <f>-SUMPRODUCT(Q16:Q19,'Proforma Inputs'!$B84:$B87)</f>
-        <v>-56249.999999999993</v>
+        <v>0</v>
       </c>
       <c r="R39" s="5">
         <f>-SUMPRODUCT(R16:R19,'Proforma Inputs'!$B84:$B87)</f>
-        <v>-56249.999999999993</v>
+        <v>0</v>
       </c>
       <c r="S39" s="5">
         <f>-SUMPRODUCT(S16:S19,'Proforma Inputs'!$B84:$B87)</f>
-        <v>-56249.999999999993</v>
+        <v>0</v>
       </c>
       <c r="T39" s="5">
         <f>-SUMPRODUCT(T16:T19,'Proforma Inputs'!$B84:$B87)</f>
-        <v>-56249.999999999993</v>
+        <v>0</v>
       </c>
       <c r="U39" s="5">
         <f>-SUMPRODUCT(U16:U19,'Proforma Inputs'!$B84:$B87)</f>
@@ -7834,59 +7834,59 @@
       </c>
       <c r="G40" s="5">
         <f>-SUMPRODUCT(G21:G27,'Proforma Inputs'!$B$108:$B$114)</f>
-        <v>-24999.999999999996</v>
+        <v>0</v>
       </c>
       <c r="H40" s="5">
         <f>-SUMPRODUCT(H21:H27,'Proforma Inputs'!$B$108:$B$114)</f>
-        <v>-49999.999999999993</v>
+        <v>0</v>
       </c>
       <c r="I40" s="5">
         <f>-SUMPRODUCT(I21:I27,'Proforma Inputs'!$B$108:$B$114)</f>
-        <v>-75000</v>
+        <v>0</v>
       </c>
       <c r="J40" s="5">
         <f>-SUMPRODUCT(J21:J27,'Proforma Inputs'!$B$108:$B$114)</f>
-        <v>-99999.999999999985</v>
+        <v>0</v>
       </c>
       <c r="K40" s="5">
         <f>-SUMPRODUCT(K21:K27,'Proforma Inputs'!$B$108:$B$114)</f>
-        <v>-124999.99999999999</v>
+        <v>0</v>
       </c>
       <c r="L40" s="5">
         <f>-SUMPRODUCT(L21:L27,'Proforma Inputs'!$B$108:$B$114)</f>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="M40" s="5">
         <f>-SUMPRODUCT(M21:M27,'Proforma Inputs'!$B$108:$B$114)</f>
-        <v>-174999.99999999997</v>
+        <v>0</v>
       </c>
       <c r="N40" s="5">
         <f>-SUMPRODUCT(N21:N27,'Proforma Inputs'!$B$108:$B$114)</f>
-        <v>-199999.99999999997</v>
+        <v>0</v>
       </c>
       <c r="O40" s="5">
         <f>-SUMPRODUCT(O21:O27,'Proforma Inputs'!$B$108:$B$114)</f>
-        <v>-199999.99999999997</v>
+        <v>0</v>
       </c>
       <c r="P40" s="5">
         <f>-SUMPRODUCT(P21:P27,'Proforma Inputs'!$B$108:$B$114)</f>
-        <v>-199999.99999999997</v>
+        <v>0</v>
       </c>
       <c r="Q40" s="5">
         <f>-SUMPRODUCT(Q21:Q27,'Proforma Inputs'!$B$108:$B$114)</f>
-        <v>-199999.99999999997</v>
+        <v>0</v>
       </c>
       <c r="R40" s="5">
         <f>-SUMPRODUCT(R21:R27,'Proforma Inputs'!$B$108:$B$114)</f>
-        <v>-199999.99999999997</v>
+        <v>0</v>
       </c>
       <c r="S40" s="5">
         <f>-SUMPRODUCT(S21:S27,'Proforma Inputs'!$B$108:$B$114)</f>
-        <v>-199999.99999999997</v>
+        <v>0</v>
       </c>
       <c r="T40" s="5">
         <f>-SUMPRODUCT(T21:T27,'Proforma Inputs'!$B$108:$B$114)</f>
-        <v>-199999.99999999997</v>
+        <v>0</v>
       </c>
       <c r="U40" s="5">
         <f>-SUMPRODUCT(U21:U27,'Proforma Inputs'!$B$108:$B$114)</f>
@@ -7992,19 +7992,19 @@
       </c>
       <c r="C41" s="5">
         <f>IF(AND(C88=0,C3&gt;='Proforma Inputs'!$B$43,C3&lt;'Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$41*'Proforma Inputs'!$B$17,0)</f>
-        <v>-50000</v>
+        <v>-1000</v>
       </c>
       <c r="D41" s="5">
         <f>IF(AND(D88=0,D3&gt;='Proforma Inputs'!$B$43,D3&lt;'Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$41*'Proforma Inputs'!$B$17,0)</f>
-        <v>-50000</v>
+        <v>-1000</v>
       </c>
       <c r="E41" s="5">
         <f>IF(AND(E88=0,E3&gt;='Proforma Inputs'!$B$43,E3&lt;'Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$41*'Proforma Inputs'!$B$17,0)</f>
-        <v>-50000</v>
+        <v>-1000</v>
       </c>
       <c r="F41" s="5">
         <f>IF(AND(F88=0,F3&gt;='Proforma Inputs'!$B$43,F3&lt;'Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$41*'Proforma Inputs'!$B$17,0)</f>
-        <v>-50000</v>
+        <v>-1000</v>
       </c>
       <c r="G41" s="5">
         <f>IF(AND(G88=0,G3&gt;='Proforma Inputs'!$B$43,G3&lt;'Proforma Inputs'!$B$44),-'Proforma Inputs'!$B$41*'Proforma Inputs'!$B$17,0)</f>
@@ -8166,19 +8166,19 @@
       </c>
       <c r="C42" s="5">
         <f>IF(C3&lt;'Proforma Inputs'!$B$44,-(1-'Proforma Inputs'!$B$5)*'Proforma Inputs'!$B$40/('Proforma Inputs'!$B$44-1),0)</f>
-        <v>-3750000</v>
+        <v>0</v>
       </c>
       <c r="D42" s="5">
         <f>IF(D3&lt;'Proforma Inputs'!$B$44,-(1-'Proforma Inputs'!$B$5)*'Proforma Inputs'!$B$40/('Proforma Inputs'!$B$44-1),0)</f>
-        <v>-3750000</v>
+        <v>0</v>
       </c>
       <c r="E42" s="5">
         <f>IF(E3&lt;'Proforma Inputs'!$B$44,-(1-'Proforma Inputs'!$B$5)*'Proforma Inputs'!$B$40/('Proforma Inputs'!$B$44-1),0)</f>
-        <v>-3750000</v>
+        <v>0</v>
       </c>
       <c r="F42" s="5">
         <f>IF(F3&lt;'Proforma Inputs'!$B$44,-(1-'Proforma Inputs'!$B$5)*'Proforma Inputs'!$B$40/('Proforma Inputs'!$B$44-1),0)</f>
-        <v>-3750000</v>
+        <v>0</v>
       </c>
       <c r="G42" s="5">
         <f>IF(G3&lt;'Proforma Inputs'!$B$44,-(1-'Proforma Inputs'!$B$5)*'Proforma Inputs'!$B$40/('Proforma Inputs'!$B$44-1),0)</f>
@@ -8340,7 +8340,7 @@
       </c>
       <c r="C43" s="5">
         <f>IF(C3=1,-'Proforma Inputs'!$B$41,0)</f>
-        <v>-5000000</v>
+        <v>-100000</v>
       </c>
       <c r="D43" s="5">
         <f>IF(D3=1,-'Proforma Inputs'!$B$41,0)</f>
@@ -8514,39 +8514,39 @@
       </c>
       <c r="C44" s="5">
         <f>B57*-'Proforma Inputs'!$B$12/'Proforma Inputs'!$B$4</f>
-        <v>-318750</v>
+        <v>0</v>
       </c>
       <c r="D44" s="5">
         <f>D57*-'Proforma Inputs'!$B$12/'Proforma Inputs'!$B$4</f>
-        <v>-318750</v>
+        <v>0</v>
       </c>
       <c r="E44" s="5">
         <f>E57*-'Proforma Inputs'!$B$12/'Proforma Inputs'!$B$4</f>
-        <v>-318750</v>
+        <v>0</v>
       </c>
       <c r="F44" s="5">
         <f>F57*-'Proforma Inputs'!$B$12/'Proforma Inputs'!$B$4</f>
-        <v>-318750</v>
+        <v>0</v>
       </c>
       <c r="G44" s="5">
         <f>G57*-'Proforma Inputs'!$B$12/'Proforma Inputs'!$B$4</f>
-        <v>-318750</v>
+        <v>0</v>
       </c>
       <c r="H44" s="5">
         <f>H57*-'Proforma Inputs'!$B$12/'Proforma Inputs'!$B$4</f>
-        <v>-244620.82985627573</v>
+        <v>0</v>
       </c>
       <c r="I44" s="5">
         <f>I57*-'Proforma Inputs'!$B$12/'Proforma Inputs'!$B$4</f>
-        <v>-187777.07985627573</v>
+        <v>0</v>
       </c>
       <c r="J44" s="5">
         <f>J57*-'Proforma Inputs'!$B$12/'Proforma Inputs'!$B$4</f>
-        <v>-116323.95485627573</v>
+        <v>0</v>
       </c>
       <c r="K44" s="5">
         <f>K57*-'Proforma Inputs'!$B$12/'Proforma Inputs'!$B$4</f>
-        <v>-30261.454856275719</v>
+        <v>0</v>
       </c>
       <c r="L44" s="5">
         <f>L57*-'Proforma Inputs'!$B$12/'Proforma Inputs'!$B$4</f>
@@ -8704,23 +8704,23 @@
       </c>
       <c r="G45" s="5">
         <f t="shared" si="3"/>
-        <v>-3488431.5361752608</v>
+        <v>0</v>
       </c>
       <c r="H45" s="5">
         <f t="shared" si="3"/>
-        <v>-2675000</v>
+        <v>0</v>
       </c>
       <c r="I45" s="5">
         <f t="shared" si="3"/>
-        <v>-3362500</v>
+        <v>0</v>
       </c>
       <c r="J45" s="5">
         <f t="shared" si="3"/>
-        <v>-4050000</v>
+        <v>0</v>
       </c>
       <c r="K45" s="5">
         <f t="shared" si="3"/>
-        <v>-1424068.4638247397</v>
+        <v>0</v>
       </c>
       <c r="L45" s="5">
         <f t="shared" si="3"/>
@@ -8877,59 +8877,59 @@
       </c>
       <c r="G46" s="17">
         <f t="shared" si="4"/>
-        <v>-112916.66666666666</v>
+        <v>0</v>
       </c>
       <c r="H46" s="17">
         <f t="shared" si="4"/>
-        <v>-112916.66666666666</v>
+        <v>0</v>
       </c>
       <c r="I46" s="17">
         <f t="shared" si="4"/>
-        <v>-112916.66666666666</v>
+        <v>0</v>
       </c>
       <c r="J46" s="17">
         <f t="shared" si="4"/>
-        <v>-112916.66666666666</v>
+        <v>0</v>
       </c>
       <c r="K46" s="17">
         <f t="shared" si="4"/>
-        <v>-112916.66666666666</v>
+        <v>0</v>
       </c>
       <c r="L46" s="17">
         <f t="shared" si="4"/>
-        <v>-112916.66666666666</v>
+        <v>0</v>
       </c>
       <c r="M46" s="17">
         <f t="shared" si="4"/>
-        <v>-112916.66666666666</v>
+        <v>0</v>
       </c>
       <c r="N46" s="17">
         <f t="shared" si="4"/>
-        <v>-112916.66666666666</v>
+        <v>0</v>
       </c>
       <c r="O46" s="17">
         <f t="shared" si="4"/>
-        <v>-112916.66666666666</v>
+        <v>0</v>
       </c>
       <c r="P46" s="17">
         <f t="shared" si="4"/>
-        <v>-112916.66666666666</v>
+        <v>0</v>
       </c>
       <c r="Q46" s="17">
         <f t="shared" si="4"/>
-        <v>-112916.66666666666</v>
+        <v>0</v>
       </c>
       <c r="R46" s="17">
         <f t="shared" si="4"/>
-        <v>-112916.66666666666</v>
+        <v>0</v>
       </c>
       <c r="S46" s="17">
         <f t="shared" si="4"/>
-        <v>-112916.66666666666</v>
+        <v>0</v>
       </c>
       <c r="T46" s="17">
         <f t="shared" si="4"/>
-        <v>-112916.66666666666</v>
+        <v>0</v>
       </c>
       <c r="U46" s="17">
         <f t="shared" si="4"/>
@@ -9103,7 +9103,7 @@
       </c>
       <c r="T47" s="17">
         <f t="shared" si="5"/>
-        <v>-1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="U47" s="17">
         <f t="shared" si="5"/>
@@ -9209,75 +9209,75 @@
       </c>
       <c r="C48" s="6">
         <f>SUM(C34:C47)</f>
-        <v>-9118750</v>
+        <v>-101000</v>
       </c>
       <c r="D48" s="6">
         <f t="shared" ref="D48:AP48" si="6">SUM(D34:D47)</f>
-        <v>-4118750</v>
+        <v>-1000</v>
       </c>
       <c r="E48" s="6">
         <f t="shared" si="6"/>
-        <v>-4118750</v>
+        <v>-1000</v>
       </c>
       <c r="F48" s="6">
         <f t="shared" si="6"/>
-        <v>-4118750</v>
+        <v>-1000</v>
       </c>
       <c r="G48" s="6">
         <f t="shared" si="6"/>
-        <v>-4466452.3695085943</v>
+        <v>-8500</v>
       </c>
       <c r="H48" s="6">
         <f t="shared" si="6"/>
-        <v>-3700245.8298562756</v>
+        <v>0</v>
       </c>
       <c r="I48" s="6">
         <f t="shared" si="6"/>
-        <v>-4452256.2465229426</v>
+        <v>0</v>
       </c>
       <c r="J48" s="6">
         <f t="shared" si="6"/>
-        <v>-5189657.2881896095</v>
+        <v>0</v>
       </c>
       <c r="K48" s="6">
         <f t="shared" si="6"/>
-        <v>-2570371.5853476818</v>
+        <v>0</v>
       </c>
       <c r="L48" s="6">
         <f t="shared" si="6"/>
-        <v>-1208750.0000000002</v>
+        <v>0</v>
       </c>
       <c r="M48" s="6">
         <f t="shared" si="6"/>
-        <v>-1301458.3333333333</v>
+        <v>0</v>
       </c>
       <c r="N48" s="6">
         <f t="shared" si="6"/>
-        <v>-1394166.6666666667</v>
+        <v>0</v>
       </c>
       <c r="O48" s="6">
         <f t="shared" si="6"/>
-        <v>-1394166.6666666667</v>
+        <v>0</v>
       </c>
       <c r="P48" s="6">
         <f t="shared" si="6"/>
-        <v>-1394166.6666666667</v>
+        <v>0</v>
       </c>
       <c r="Q48" s="6">
         <f t="shared" si="6"/>
-        <v>-1394166.6666666667</v>
+        <v>0</v>
       </c>
       <c r="R48" s="6">
         <f t="shared" si="6"/>
-        <v>-1394166.6666666667</v>
+        <v>0</v>
       </c>
       <c r="S48" s="6">
         <f t="shared" si="6"/>
-        <v>-1394166.6666666667</v>
+        <v>0</v>
       </c>
       <c r="T48" s="6">
         <f t="shared" si="6"/>
-        <v>-2895098.2028419273</v>
+        <v>0</v>
       </c>
       <c r="U48" s="6">
         <f t="shared" si="6"/>
@@ -9432,75 +9432,75 @@
       </c>
       <c r="C50" s="13">
         <f t="shared" ref="C50:AP50" si="7">C31+C48</f>
-        <v>-9118750</v>
+        <v>-101000</v>
       </c>
       <c r="D50" s="13">
         <f t="shared" si="7"/>
-        <v>-4118750</v>
+        <v>-1000</v>
       </c>
       <c r="E50" s="13">
         <f t="shared" si="7"/>
-        <v>-4118750</v>
+        <v>-1000</v>
       </c>
       <c r="F50" s="13">
         <f t="shared" si="7"/>
-        <v>-4118750</v>
+        <v>-1000</v>
       </c>
       <c r="G50" s="13">
         <f t="shared" si="7"/>
-        <v>-978020.83333333349</v>
+        <v>-129928.57142857142</v>
       </c>
       <c r="H50" s="13">
         <f t="shared" si="7"/>
-        <v>-1025245.8298562756</v>
+        <v>0</v>
       </c>
       <c r="I50" s="13">
         <f t="shared" si="7"/>
-        <v>-1089756.2465229426</v>
+        <v>0</v>
       </c>
       <c r="J50" s="13">
         <f t="shared" si="7"/>
-        <v>-1139657.2881896095</v>
+        <v>0</v>
       </c>
       <c r="K50" s="13">
         <f t="shared" si="7"/>
-        <v>2042128.4146523182</v>
+        <v>0</v>
       </c>
       <c r="L50" s="13">
         <f t="shared" si="7"/>
-        <v>3966250</v>
+        <v>0</v>
       </c>
       <c r="M50" s="13">
         <f t="shared" si="7"/>
-        <v>4436041.666666667</v>
+        <v>0</v>
       </c>
       <c r="N50" s="13">
         <f t="shared" si="7"/>
-        <v>4905833.333333333</v>
+        <v>0</v>
       </c>
       <c r="O50" s="13">
         <f t="shared" si="7"/>
-        <v>4655833.333333333</v>
+        <v>0</v>
       </c>
       <c r="P50" s="13">
         <f t="shared" si="7"/>
-        <v>4655833.333333333</v>
+        <v>0</v>
       </c>
       <c r="Q50" s="13">
         <f t="shared" si="7"/>
-        <v>4355833.333333333</v>
+        <v>0</v>
       </c>
       <c r="R50" s="13">
         <f t="shared" si="7"/>
-        <v>4155833.333333333</v>
+        <v>0</v>
       </c>
       <c r="S50" s="13">
         <f t="shared" si="7"/>
-        <v>3805833.333333333</v>
+        <v>0</v>
       </c>
       <c r="T50" s="13">
         <f t="shared" si="7"/>
-        <v>55229901.797158062</v>
+        <v>0</v>
       </c>
       <c r="U50" s="13">
         <f t="shared" si="7"/>
@@ -9652,7 +9652,7 @@
       </c>
       <c r="B52" s="5">
         <f>NPV('Proforma Inputs'!$B$13,C50:AP50)</f>
-        <v>-7176521.0644891392</v>
+        <v>-154408.96306667136</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -9908,43 +9908,43 @@
       </c>
       <c r="B57" s="5">
         <f>'Proforma Inputs'!B5*'Proforma Inputs'!B40</f>
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="C57" s="5">
         <f>B57+B45</f>
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="D57" s="5">
         <f>C57+C45</f>
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="E57" s="5">
         <f t="shared" ref="E57:AP57" si="8">D57+D45</f>
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="F57" s="5">
         <f t="shared" si="8"/>
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="G57" s="5">
         <f t="shared" si="8"/>
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="H57" s="5">
         <f t="shared" si="8"/>
-        <v>11511568.46382474</v>
+        <v>0</v>
       </c>
       <c r="I57" s="5">
         <f t="shared" si="8"/>
-        <v>8836568.4638247397</v>
+        <v>0</v>
       </c>
       <c r="J57" s="5">
         <f t="shared" si="8"/>
-        <v>5474068.4638247397</v>
+        <v>0</v>
       </c>
       <c r="K57" s="5">
         <f t="shared" si="8"/>
-        <v>1424068.4638247397</v>
+        <v>0</v>
       </c>
       <c r="L57" s="5">
         <f t="shared" si="8"/>
@@ -10135,55 +10135,55 @@
       </c>
       <c r="B59" s="17">
         <f>'Proforma Inputs'!B48</f>
-        <v>2000000</v>
+        <v>0</v>
       </c>
       <c r="C59" s="17">
         <f t="shared" ref="C59:AP59" si="9">B59-B6</f>
-        <v>2000000</v>
+        <v>0</v>
       </c>
       <c r="D59" s="17">
         <f t="shared" si="9"/>
-        <v>2000000</v>
+        <v>0</v>
       </c>
       <c r="E59" s="17">
         <f t="shared" si="9"/>
-        <v>2000000</v>
+        <v>0</v>
       </c>
       <c r="F59" s="17">
         <f t="shared" si="9"/>
-        <v>2000000</v>
+        <v>0</v>
       </c>
       <c r="G59" s="17">
         <f t="shared" si="9"/>
-        <v>2000000</v>
+        <v>0</v>
       </c>
       <c r="H59" s="17">
         <f t="shared" si="9"/>
-        <v>1750000</v>
+        <v>0</v>
       </c>
       <c r="I59" s="17">
         <f t="shared" si="9"/>
-        <v>1500000</v>
+        <v>0</v>
       </c>
       <c r="J59" s="17">
         <f t="shared" si="9"/>
-        <v>1250000</v>
+        <v>0</v>
       </c>
       <c r="K59" s="17">
         <f t="shared" si="9"/>
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="L59" s="17">
         <f t="shared" si="9"/>
-        <v>750000</v>
+        <v>0</v>
       </c>
       <c r="M59" s="17">
         <f t="shared" si="9"/>
-        <v>500000</v>
+        <v>0</v>
       </c>
       <c r="N59" s="17">
         <f t="shared" si="9"/>
-        <v>250000</v>
+        <v>0</v>
       </c>
       <c r="O59" s="17">
         <f t="shared" si="9"/>
@@ -10310,63 +10310,63 @@
       </c>
       <c r="B60" s="17">
         <f>'Proforma Inputs'!B49</f>
-        <v>3000000</v>
+        <v>0</v>
       </c>
       <c r="C60" s="17">
         <f t="shared" ref="C60:AP60" si="10">B60-B7</f>
-        <v>3000000</v>
+        <v>0</v>
       </c>
       <c r="D60" s="17">
         <f t="shared" si="10"/>
-        <v>3000000</v>
+        <v>0</v>
       </c>
       <c r="E60" s="17">
         <f t="shared" si="10"/>
-        <v>3000000</v>
+        <v>0</v>
       </c>
       <c r="F60" s="17">
         <f t="shared" si="10"/>
-        <v>3000000</v>
+        <v>0</v>
       </c>
       <c r="G60" s="17">
         <f t="shared" si="10"/>
-        <v>3000000</v>
+        <v>0</v>
       </c>
       <c r="H60" s="17">
         <f t="shared" si="10"/>
-        <v>2700000</v>
+        <v>0</v>
       </c>
       <c r="I60" s="17">
         <f t="shared" si="10"/>
-        <v>2400000</v>
+        <v>0</v>
       </c>
       <c r="J60" s="17">
         <f t="shared" si="10"/>
-        <v>2100000</v>
+        <v>0</v>
       </c>
       <c r="K60" s="17">
         <f t="shared" si="10"/>
-        <v>1800000</v>
+        <v>0</v>
       </c>
       <c r="L60" s="17">
         <f t="shared" si="10"/>
-        <v>1500000</v>
+        <v>0</v>
       </c>
       <c r="M60" s="17">
         <f t="shared" si="10"/>
-        <v>1200000</v>
+        <v>0</v>
       </c>
       <c r="N60" s="17">
         <f t="shared" si="10"/>
-        <v>900000</v>
+        <v>0</v>
       </c>
       <c r="O60" s="17">
         <f t="shared" si="10"/>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="P60" s="17">
         <f t="shared" si="10"/>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="Q60" s="17">
         <f t="shared" si="10"/>
@@ -10485,71 +10485,71 @@
       </c>
       <c r="B61" s="17">
         <f>'Proforma Inputs'!B50</f>
-        <v>4000000</v>
+        <v>0</v>
       </c>
       <c r="C61" s="17">
         <f t="shared" ref="C61:AP61" si="11">B61-B8</f>
-        <v>4000000</v>
+        <v>0</v>
       </c>
       <c r="D61" s="17">
         <f t="shared" si="11"/>
-        <v>4000000</v>
+        <v>0</v>
       </c>
       <c r="E61" s="17">
         <f t="shared" si="11"/>
-        <v>4000000</v>
+        <v>0</v>
       </c>
       <c r="F61" s="17">
         <f t="shared" si="11"/>
-        <v>4000000</v>
+        <v>0</v>
       </c>
       <c r="G61" s="17">
         <f t="shared" si="11"/>
-        <v>4000000</v>
+        <v>0</v>
       </c>
       <c r="H61" s="17">
         <f t="shared" si="11"/>
-        <v>3650000</v>
+        <v>0</v>
       </c>
       <c r="I61" s="17">
         <f t="shared" si="11"/>
-        <v>3300000</v>
+        <v>0</v>
       </c>
       <c r="J61" s="17">
         <f t="shared" si="11"/>
-        <v>2950000</v>
+        <v>0</v>
       </c>
       <c r="K61" s="17">
         <f t="shared" si="11"/>
-        <v>2600000</v>
+        <v>0</v>
       </c>
       <c r="L61" s="17">
         <f t="shared" si="11"/>
-        <v>2250000</v>
+        <v>0</v>
       </c>
       <c r="M61" s="17">
         <f t="shared" si="11"/>
-        <v>1900000</v>
+        <v>0</v>
       </c>
       <c r="N61" s="17">
         <f t="shared" si="11"/>
-        <v>1550000</v>
+        <v>0</v>
       </c>
       <c r="O61" s="17">
         <f t="shared" si="11"/>
-        <v>1200000</v>
+        <v>0</v>
       </c>
       <c r="P61" s="17">
         <f t="shared" si="11"/>
-        <v>850000</v>
+        <v>0</v>
       </c>
       <c r="Q61" s="17">
         <f t="shared" si="11"/>
-        <v>500000</v>
+        <v>0</v>
       </c>
       <c r="R61" s="17">
         <f t="shared" si="11"/>
-        <v>150000</v>
+        <v>0</v>
       </c>
       <c r="S61" s="17">
         <f t="shared" si="11"/>
@@ -10660,75 +10660,75 @@
       </c>
       <c r="B62" s="17">
         <f>'Proforma Inputs'!B51</f>
-        <v>5000000</v>
+        <v>0</v>
       </c>
       <c r="C62" s="17">
         <f t="shared" ref="C62:AP62" si="12">B62-B9</f>
-        <v>5000000</v>
+        <v>0</v>
       </c>
       <c r="D62" s="17">
         <f t="shared" si="12"/>
-        <v>5000000</v>
+        <v>0</v>
       </c>
       <c r="E62" s="17">
         <f t="shared" si="12"/>
-        <v>5000000</v>
+        <v>0</v>
       </c>
       <c r="F62" s="17">
         <f t="shared" si="12"/>
-        <v>5000000</v>
+        <v>0</v>
       </c>
       <c r="G62" s="17">
         <f t="shared" si="12"/>
-        <v>5000000</v>
+        <v>0</v>
       </c>
       <c r="H62" s="17">
         <f t="shared" si="12"/>
-        <v>4600000</v>
+        <v>0</v>
       </c>
       <c r="I62" s="17">
         <f t="shared" si="12"/>
-        <v>4200000</v>
+        <v>0</v>
       </c>
       <c r="J62" s="17">
         <f t="shared" si="12"/>
-        <v>3800000</v>
+        <v>0</v>
       </c>
       <c r="K62" s="17">
         <f t="shared" si="12"/>
-        <v>3400000</v>
+        <v>0</v>
       </c>
       <c r="L62" s="17">
         <f t="shared" si="12"/>
-        <v>3000000</v>
+        <v>0</v>
       </c>
       <c r="M62" s="17">
         <f t="shared" si="12"/>
-        <v>2600000</v>
+        <v>0</v>
       </c>
       <c r="N62" s="17">
         <f t="shared" si="12"/>
-        <v>2200000</v>
+        <v>0</v>
       </c>
       <c r="O62" s="17">
         <f t="shared" si="12"/>
-        <v>1800000</v>
+        <v>0</v>
       </c>
       <c r="P62" s="17">
         <f t="shared" si="12"/>
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="Q62" s="17">
         <f t="shared" si="12"/>
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="R62" s="17">
         <f t="shared" si="12"/>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="S62" s="17">
         <f t="shared" si="12"/>
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="T62" s="17">
         <f t="shared" si="12"/>
@@ -11589,163 +11589,163 @@
         <v>0</v>
       </c>
       <c r="C68" s="15">
-        <f>IF(SUM(C16:C27,C35:C40)&gt;0,IF(SUM($B$68:B68)=1,0,IF(SUM(C16:C27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(C16:C27,C35:C40)&gt;0,IF(SUM($B$68:B68)=1,0,IF(SUM(C16:C27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="D68" s="15">
-        <f>IF(SUM(D16:D27,D35:D40)&gt;0,IF(SUM($B$68:C68)=1,0,IF(SUM(D16:D27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(D16:D27,D35:D40)&gt;0,IF(SUM($B$68:C68)=1,0,IF(SUM(D16:D27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="E68" s="15">
-        <f>IF(SUM(E16:E27,E35:E40)&gt;0,IF(SUM($B$68:D68)=1,0,IF(SUM(E16:E27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(E16:E27,E35:E40)&gt;0,IF(SUM($B$68:D68)=1,0,IF(SUM(E16:E27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="F68" s="15">
-        <f>IF(SUM(F16:F27,F35:F40)&gt;0,IF(SUM($B$68:E68)=1,0,IF(SUM(F16:F27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(F16:F27,F35:F40)&gt;0,IF(SUM($B$68:E68)=1,0,IF(SUM(F16:F27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="G68" s="15">
-        <f>IF(SUM(G16:G27,G35:G40)&gt;0,IF(SUM($B$68:F68)=1,0,IF(SUM(G16:G27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
-        <v>1</v>
+        <f>IF(SUM(G16:G27,G35:G40)&gt;0,IF(SUM($B$68:F68)=1,0,IF(SUM(G16:G27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
+        <v>0</v>
       </c>
       <c r="H68" s="15">
-        <f>IF(SUM(H16:H27,H35:H40)&gt;0,IF(SUM($B$68:G68)=1,0,IF(SUM(H16:H27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(H16:H27,H35:H40)&gt;0,IF(SUM($B$68:G68)=1,0,IF(SUM(H16:H27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="I68" s="15">
-        <f>IF(SUM(I16:I27,I35:I40)&gt;0,IF(SUM($B$68:H68)=1,0,IF(SUM(I16:I27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(I16:I27,I35:I40)&gt;0,IF(SUM($B$68:H68)=1,0,IF(SUM(I16:I27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="J68" s="15">
-        <f>IF(SUM(J16:J27,J35:J40)&gt;0,IF(SUM($B$68:I68)=1,0,IF(SUM(J16:J27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(J16:J27,J35:J40)&gt;0,IF(SUM($B$68:I68)=1,0,IF(SUM(J16:J27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="K68" s="15">
-        <f>IF(SUM(K16:K27,K35:K40)&gt;0,IF(SUM($B$68:J68)=1,0,IF(SUM(K16:K27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(K16:K27,K35:K40)&gt;0,IF(SUM($B$68:J68)=1,0,IF(SUM(K16:K27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="L68" s="15">
-        <f>IF(SUM(L16:L27,L35:L40)&gt;0,IF(SUM($B$68:K68)=1,0,IF(SUM(L16:L27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(L16:L27,L35:L40)&gt;0,IF(SUM($B$68:K68)=1,0,IF(SUM(L16:L27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="M68" s="15">
-        <f>IF(SUM(M16:M27,M35:M40)&gt;0,IF(SUM($B$68:L68)=1,0,IF(SUM(M16:M27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(M16:M27,M35:M40)&gt;0,IF(SUM($B$68:L68)=1,0,IF(SUM(M16:M27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="N68" s="15">
-        <f>IF(SUM(N16:N27,N35:N40)&gt;0,IF(SUM($B$68:M68)=1,0,IF(SUM(N16:N27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(N16:N27,N35:N40)&gt;0,IF(SUM($B$68:M68)=1,0,IF(SUM(N16:N27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="O68" s="15">
-        <f>IF(SUM(O16:O27,O35:O40)&gt;0,IF(SUM($B$68:N68)=1,0,IF(SUM(O16:O27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(O16:O27,O35:O40)&gt;0,IF(SUM($B$68:N68)=1,0,IF(SUM(O16:O27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="P68" s="15">
-        <f>IF(SUM(P16:P27,P35:P40)&gt;0,IF(SUM($B$68:O68)=1,0,IF(SUM(P16:P27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(P16:P27,P35:P40)&gt;0,IF(SUM($B$68:O68)=1,0,IF(SUM(P16:P27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="Q68" s="15">
-        <f>IF(SUM(Q16:Q27,Q35:Q40)&gt;0,IF(SUM($B$68:P68)=1,0,IF(SUM(Q16:Q27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(Q16:Q27,Q35:Q40)&gt;0,IF(SUM($B$68:P68)=1,0,IF(SUM(Q16:Q27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="R68" s="15">
-        <f>IF(SUM(R16:R27,R35:R40)&gt;0,IF(SUM($B$68:Q68)=1,0,IF(SUM(R16:R27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(R16:R27,R35:R40)&gt;0,IF(SUM($B$68:Q68)=1,0,IF(SUM(R16:R27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="S68" s="15">
-        <f>IF(SUM(S16:S27,S35:S40)&gt;0,IF(SUM($B$68:R68)=1,0,IF(SUM(S16:S27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(S16:S27,S35:S40)&gt;0,IF(SUM($B$68:R68)=1,0,IF(SUM(S16:S27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="T68" s="15">
-        <f>IF(SUM(T16:T27,T35:T40)&gt;0,IF(SUM($B$68:S68)=1,0,IF(SUM(T16:T27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(T16:T27,T35:T40)&gt;0,IF(SUM($B$68:S68)=1,0,IF(SUM(T16:T27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="U68" s="15">
-        <f>IF(SUM(U16:U27,U35:U40)&gt;0,IF(SUM($B$68:T68)=1,0,IF(SUM(U16:U27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(U16:U27,U35:U40)&gt;0,IF(SUM($B$68:T68)=1,0,IF(SUM(U16:U27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="V68" s="15">
-        <f>IF(SUM(V16:V27,V35:V40)&gt;0,IF(SUM($B$68:U68)=1,0,IF(SUM(V16:V27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(V16:V27,V35:V40)&gt;0,IF(SUM($B$68:U68)=1,0,IF(SUM(V16:V27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="W68" s="15">
-        <f>IF(SUM(W16:W27,W35:W40)&gt;0,IF(SUM($B$68:V68)=1,0,IF(SUM(W16:W27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(W16:W27,W35:W40)&gt;0,IF(SUM($B$68:V68)=1,0,IF(SUM(W16:W27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="X68" s="15">
-        <f>IF(SUM(X16:X27,X35:X40)&gt;0,IF(SUM($B$68:W68)=1,0,IF(SUM(X16:X27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(X16:X27,X35:X40)&gt;0,IF(SUM($B$68:W68)=1,0,IF(SUM(X16:X27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="Y68" s="15">
-        <f>IF(SUM(Y16:Y27,Y35:Y40)&gt;0,IF(SUM($B$68:X68)=1,0,IF(SUM(Y16:Y27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(Y16:Y27,Y35:Y40)&gt;0,IF(SUM($B$68:X68)=1,0,IF(SUM(Y16:Y27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="Z68" s="15">
-        <f>IF(SUM(Z16:Z27,Z35:Z40)&gt;0,IF(SUM($B$68:Y68)=1,0,IF(SUM(Z16:Z27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(Z16:Z27,Z35:Z40)&gt;0,IF(SUM($B$68:Y68)=1,0,IF(SUM(Z16:Z27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="AA68" s="15">
-        <f>IF(SUM(AA16:AA27,AA35:AA40)&gt;0,IF(SUM($B$68:Z68)=1,0,IF(SUM(AA16:AA27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(AA16:AA27,AA35:AA40)&gt;0,IF(SUM($B$68:Z68)=1,0,IF(SUM(AA16:AA27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="AB68" s="15">
-        <f>IF(SUM(AB16:AB27,AB35:AB40)&gt;0,IF(SUM($B$68:AA68)=1,0,IF(SUM(AB16:AB27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(AB16:AB27,AB35:AB40)&gt;0,IF(SUM($B$68:AA68)=1,0,IF(SUM(AB16:AB27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="AC68" s="15">
-        <f>IF(SUM(AC16:AC27,AC35:AC40)&gt;0,IF(SUM($B$68:AB68)=1,0,IF(SUM(AC16:AC27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(AC16:AC27,AC35:AC40)&gt;0,IF(SUM($B$68:AB68)=1,0,IF(SUM(AC16:AC27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="AD68" s="15">
-        <f>IF(SUM(AD16:AD27,AD35:AD40)&gt;0,IF(SUM($B$68:AC68)=1,0,IF(SUM(AD16:AD27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(AD16:AD27,AD35:AD40)&gt;0,IF(SUM($B$68:AC68)=1,0,IF(SUM(AD16:AD27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="AE68" s="15">
-        <f>IF(SUM(AE16:AE27,AE35:AE40)&gt;0,IF(SUM($B$68:AD68)=1,0,IF(SUM(AE16:AE27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(AE16:AE27,AE35:AE40)&gt;0,IF(SUM($B$68:AD68)=1,0,IF(SUM(AE16:AE27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="AF68" s="15">
-        <f>IF(SUM(AF16:AF27,AF35:AF40)&gt;0,IF(SUM($B$68:AE68)=1,0,IF(SUM(AF16:AF27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(AF16:AF27,AF35:AF40)&gt;0,IF(SUM($B$68:AE68)=1,0,IF(SUM(AF16:AF27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="AG68" s="15">
-        <f>IF(SUM(AG16:AG27,AG35:AG40)&gt;0,IF(SUM($B$68:AF68)=1,0,IF(SUM(AG16:AG27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(AG16:AG27,AG35:AG40)&gt;0,IF(SUM($B$68:AF68)=1,0,IF(SUM(AG16:AG27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="AH68" s="15">
-        <f>IF(SUM(AH16:AH27,AH35:AH40)&gt;0,IF(SUM($B$68:AG68)=1,0,IF(SUM(AH16:AH27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(AH16:AH27,AH35:AH40)&gt;0,IF(SUM($B$68:AG68)=1,0,IF(SUM(AH16:AH27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="AI68" s="15">
-        <f>IF(SUM(AI16:AI27,AI35:AI40)&gt;0,IF(SUM($B$68:AH68)=1,0,IF(SUM(AI16:AI27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(AI16:AI27,AI35:AI40)&gt;0,IF(SUM($B$68:AH68)=1,0,IF(SUM(AI16:AI27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="AJ68" s="15">
-        <f>IF(SUM(AJ16:AJ27,AJ35:AJ40)&gt;0,IF(SUM($B$68:AI68)=1,0,IF(SUM(AJ16:AJ27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(AJ16:AJ27,AJ35:AJ40)&gt;0,IF(SUM($B$68:AI68)=1,0,IF(SUM(AJ16:AJ27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="AK68" s="15">
-        <f>IF(SUM(AK16:AK27,AK35:AK40)&gt;0,IF(SUM($B$68:AJ68)=1,0,IF(SUM(AK16:AK27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(AK16:AK27,AK35:AK40)&gt;0,IF(SUM($B$68:AJ68)=1,0,IF(SUM(AK16:AK27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="AL68" s="15">
-        <f>IF(SUM(AL16:AL27,AL35:AL40)&gt;0,IF(SUM($B$68:AK68)=1,0,IF(SUM(AL16:AL27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(AL16:AL27,AL35:AL40)&gt;0,IF(SUM($B$68:AK68)=1,0,IF(SUM(AL16:AL27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="AM68" s="15">
-        <f>IF(SUM(AM16:AM27,AM35:AM40)&gt;0,IF(SUM($B$68:AL68)=1,0,IF(SUM(AM16:AM27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(AM16:AM27,AM35:AM40)&gt;0,IF(SUM($B$68:AL68)=1,0,IF(SUM(AM16:AM27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="AN68" s="15">
-        <f>IF(SUM(AN16:AN27,AN35:AN40)&gt;0,IF(SUM($B$68:AM68)=1,0,IF(SUM(AN16:AN27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(AN16:AN27,AN35:AN40)&gt;0,IF(SUM($B$68:AM68)=1,0,IF(SUM(AN16:AN27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="AO68" s="15">
-        <f>IF(SUM(AO16:AO27,AO35:AO40)&gt;0,IF(SUM($B$68:AN68)=1,0,IF(SUM(AO16:AO27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(AO16:AO27,AO35:AO40)&gt;0,IF(SUM($B$68:AN68)=1,0,IF(SUM(AO16:AO27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="AP68" s="15">
-        <f>IF(SUM(AP16:AP27,AP35:AP40)&gt;0,IF(SUM($B$68:AO68)=1,0,IF(SUM(AP16:AP27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$75,$B$85:$B$91),1,0)),0)</f>
+        <f>IF(SUM(AP16:AP27,AP35:AP40)&gt;0,IF(SUM($B$68:AO68)=1,0,IF(SUM(AP16:AP27)&gt;='Proforma Inputs'!$B$7*SUM('Proforma Inputs'!$B$74:$B$77,'Proforma Inputs'!$B$92:$B$98),1,0)),0)</f>
         <v>0</v>
       </c>
       <c r="AQ68" s="15"/>
@@ -11780,59 +11780,59 @@
       </c>
       <c r="G69" s="5">
         <f>G90/'Proforma Inputs'!$B$14*'Proforma Inputs'!$B$29</f>
-        <v>1512276.7857142857</v>
+        <v>-91071.428571428565</v>
       </c>
       <c r="H69" s="5">
         <f>H90/'Proforma Inputs'!$B$14*'Proforma Inputs'!$B$29</f>
-        <v>7578125</v>
+        <v>0</v>
       </c>
       <c r="I69" s="5">
         <f>I90/'Proforma Inputs'!$B$14*'Proforma Inputs'!$B$29</f>
-        <v>13643973.214285713</v>
+        <v>0</v>
       </c>
       <c r="J69" s="5">
         <f>J90/'Proforma Inputs'!$B$14*'Proforma Inputs'!$B$29</f>
-        <v>19709821.428571425</v>
+        <v>0</v>
       </c>
       <c r="K69" s="5">
         <f>K90/'Proforma Inputs'!$B$14*'Proforma Inputs'!$B$29</f>
-        <v>24743303.571428567</v>
+        <v>0</v>
       </c>
       <c r="L69" s="5">
         <f>L90/'Proforma Inputs'!$B$14*'Proforma Inputs'!$B$29</f>
-        <v>29776785.714285709</v>
+        <v>0</v>
       </c>
       <c r="M69" s="5">
         <f>M90/'Proforma Inputs'!$B$14*'Proforma Inputs'!$B$29</f>
-        <v>34810267.857142858</v>
+        <v>0</v>
       </c>
       <c r="N69" s="5">
         <f>N90/'Proforma Inputs'!$B$14*'Proforma Inputs'!$B$29</f>
-        <v>39843749.999999993</v>
+        <v>0</v>
       </c>
       <c r="O69" s="5">
         <f>O90/'Proforma Inputs'!$B$14*'Proforma Inputs'!$B$29</f>
-        <v>39843749.999999993</v>
+        <v>0</v>
       </c>
       <c r="P69" s="5">
         <f>P90/'Proforma Inputs'!$B$14*'Proforma Inputs'!$B$29</f>
-        <v>39843749.999999993</v>
+        <v>0</v>
       </c>
       <c r="Q69" s="5">
         <f>Q90/'Proforma Inputs'!$B$14*'Proforma Inputs'!$B$29</f>
-        <v>39843749.999999993</v>
+        <v>0</v>
       </c>
       <c r="R69" s="5">
         <f>R90/'Proforma Inputs'!$B$14*'Proforma Inputs'!$B$29</f>
-        <v>39843749.999999993</v>
+        <v>0</v>
       </c>
       <c r="S69" s="5">
         <f>S90/'Proforma Inputs'!$B$14*'Proforma Inputs'!$B$29</f>
-        <v>39843749.999999993</v>
+        <v>0</v>
       </c>
       <c r="T69" s="5">
         <f>T90/'Proforma Inputs'!$B$14*'Proforma Inputs'!$B$29</f>
-        <v>39843749.999999993</v>
+        <v>0</v>
       </c>
       <c r="U69" s="5">
         <f>U90/'Proforma Inputs'!$B$14*'Proforma Inputs'!$B$29</f>
@@ -11954,59 +11954,59 @@
       </c>
       <c r="G70" s="5">
         <f>-PV('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,Proforma!G90/'Proforma Inputs'!$B$30)</f>
-        <v>1500931.5361752608</v>
+        <v>-90388.201735720504</v>
       </c>
       <c r="H70" s="5">
         <f>-PV('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,Proforma!H90/'Proforma Inputs'!$B$30)</f>
-        <v>7521273.1591365458</v>
+        <v>0</v>
       </c>
       <c r="I70" s="5">
         <f>-PV('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,Proforma!I90/'Proforma Inputs'!$B$30)</f>
-        <v>13541614.782097833</v>
+        <v>0</v>
       </c>
       <c r="J70" s="5">
         <f>-PV('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,Proforma!J90/'Proforma Inputs'!$B$30)</f>
-        <v>19561956.405059114</v>
+        <v>0</v>
       </c>
       <c r="K70" s="5">
         <f>-PV('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,Proforma!K90/'Proforma Inputs'!$B$30)</f>
-        <v>24557676.868638769</v>
+        <v>0</v>
       </c>
       <c r="L70" s="5">
         <f>-PV('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,Proforma!L90/'Proforma Inputs'!$B$30)</f>
-        <v>29553397.332218412</v>
+        <v>0</v>
       </c>
       <c r="M70" s="5">
         <f>-PV('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,Proforma!M90/'Proforma Inputs'!$B$30)</f>
-        <v>34549117.795798078</v>
+        <v>0</v>
       </c>
       <c r="N70" s="5">
         <f>-PV('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,Proforma!N90/'Proforma Inputs'!$B$30)</f>
-        <v>39544838.259377725</v>
+        <v>0</v>
       </c>
       <c r="O70" s="5">
         <f>-PV('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,Proforma!O90/'Proforma Inputs'!$B$30)</f>
-        <v>39544838.259377725</v>
+        <v>0</v>
       </c>
       <c r="P70" s="5">
         <f>-PV('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,Proforma!P90/'Proforma Inputs'!$B$30)</f>
-        <v>39544838.259377725</v>
+        <v>0</v>
       </c>
       <c r="Q70" s="5">
         <f>-PV('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,Proforma!Q90/'Proforma Inputs'!$B$30)</f>
-        <v>39544838.259377725</v>
+        <v>0</v>
       </c>
       <c r="R70" s="5">
         <f>-PV('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,Proforma!R90/'Proforma Inputs'!$B$30)</f>
-        <v>39544838.259377725</v>
+        <v>0</v>
       </c>
       <c r="S70" s="5">
         <f>-PV('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,Proforma!S90/'Proforma Inputs'!$B$30)</f>
-        <v>39544838.259377725</v>
+        <v>0</v>
       </c>
       <c r="T70" s="5">
         <f>-PV('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,Proforma!T90/'Proforma Inputs'!$B$30)</f>
-        <v>39544838.259377725</v>
+        <v>0</v>
       </c>
       <c r="U70" s="5">
         <f>-PV('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,Proforma!U90/'Proforma Inputs'!$B$30)</f>
@@ -12128,59 +12128,59 @@
       </c>
       <c r="G71" s="5">
         <f t="shared" si="17"/>
-        <v>1500931.5361752608</v>
+        <v>-91071.428571428565</v>
       </c>
       <c r="H71" s="5">
         <f t="shared" si="17"/>
-        <v>7521273.1591365458</v>
+        <v>0</v>
       </c>
       <c r="I71" s="5">
         <f t="shared" ref="I71:AP71" si="18">MIN(I69:I70)</f>
-        <v>13541614.782097833</v>
+        <v>0</v>
       </c>
       <c r="J71" s="5">
         <f t="shared" si="18"/>
-        <v>19561956.405059114</v>
+        <v>0</v>
       </c>
       <c r="K71" s="5">
         <f t="shared" si="18"/>
-        <v>24557676.868638769</v>
+        <v>0</v>
       </c>
       <c r="L71" s="5">
         <f t="shared" si="18"/>
-        <v>29553397.332218412</v>
+        <v>0</v>
       </c>
       <c r="M71" s="5">
         <f t="shared" si="18"/>
-        <v>34549117.795798078</v>
+        <v>0</v>
       </c>
       <c r="N71" s="5">
         <f t="shared" si="18"/>
-        <v>39544838.259377725</v>
+        <v>0</v>
       </c>
       <c r="O71" s="5">
         <f t="shared" si="18"/>
-        <v>39544838.259377725</v>
+        <v>0</v>
       </c>
       <c r="P71" s="5">
         <f t="shared" si="18"/>
-        <v>39544838.259377725</v>
+        <v>0</v>
       </c>
       <c r="Q71" s="5">
         <f t="shared" si="18"/>
-        <v>39544838.259377725</v>
+        <v>0</v>
       </c>
       <c r="R71" s="5">
         <f t="shared" si="18"/>
-        <v>39544838.259377725</v>
+        <v>0</v>
       </c>
       <c r="S71" s="5">
         <f t="shared" si="18"/>
-        <v>39544838.259377725</v>
+        <v>0</v>
       </c>
       <c r="T71" s="5">
         <f t="shared" si="18"/>
-        <v>39544838.259377725</v>
+        <v>0</v>
       </c>
       <c r="U71" s="5">
         <f t="shared" si="18"/>
@@ -12302,59 +12302,59 @@
       </c>
       <c r="G72" s="5">
         <f>PMT('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,G71)</f>
-        <v>-112916.66666666666</v>
+        <v>6851.3998773468111</v>
       </c>
       <c r="H72" s="5">
         <f>PMT('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,H71)</f>
-        <v>-565833.33333333326</v>
+        <v>0</v>
       </c>
       <c r="I72" s="5">
         <f>PMT('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,I71)</f>
-        <v>-1018750</v>
+        <v>0</v>
       </c>
       <c r="J72" s="5">
         <f>PMT('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,J71)</f>
-        <v>-1471666.6666666665</v>
+        <v>0</v>
       </c>
       <c r="K72" s="5">
         <f>PMT('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,K71)</f>
-        <v>-1847500.0000000002</v>
+        <v>0</v>
       </c>
       <c r="L72" s="5">
         <f>PMT('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,L71)</f>
-        <v>-2223333.333333333</v>
+        <v>0</v>
       </c>
       <c r="M72" s="5">
         <f>PMT('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,M71)</f>
-        <v>-2599166.6666666674</v>
+        <v>0</v>
       </c>
       <c r="N72" s="5">
         <f>PMT('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,N71)</f>
-        <v>-2975000.0000000005</v>
+        <v>0</v>
       </c>
       <c r="O72" s="5">
         <f>PMT('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,O71)</f>
-        <v>-2975000.0000000005</v>
+        <v>0</v>
       </c>
       <c r="P72" s="5">
         <f>PMT('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,P71)</f>
-        <v>-2975000.0000000005</v>
+        <v>0</v>
       </c>
       <c r="Q72" s="5">
         <f>PMT('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,Q71)</f>
-        <v>-2975000.0000000005</v>
+        <v>0</v>
       </c>
       <c r="R72" s="5">
         <f>PMT('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,R71)</f>
-        <v>-2975000.0000000005</v>
+        <v>0</v>
       </c>
       <c r="S72" s="5">
         <f>PMT('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,S71)</f>
-        <v>-2975000.0000000005</v>
+        <v>0</v>
       </c>
       <c r="T72" s="5">
         <f>PMT('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,T71)</f>
-        <v>-2975000.0000000005</v>
+        <v>0</v>
       </c>
       <c r="U72" s="5">
         <f>PMT('Proforma Inputs'!$B$31,'Proforma Inputs'!$B$32*'Proforma Inputs'!$B$4,U71)</f>
@@ -12476,147 +12476,147 @@
       </c>
       <c r="G73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="H73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="I73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="J73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="K73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="L73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="M73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="N73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="O73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="P73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="Q73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="R73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="S73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="T73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="U73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="V73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="W73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="X73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="Y73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="Z73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="AA73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="AB73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="AC73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="AD73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="AE73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="AF73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="AG73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="AH73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="AI73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="AJ73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="AK73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="AL73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="AM73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="AN73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="AO73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="AP73" s="5">
         <f t="shared" si="19"/>
-        <v>1500931.5361752608</v>
+        <v>0</v>
       </c>
       <c r="AQ73" s="5"/>
       <c r="AR73" s="5"/>
@@ -12634,163 +12634,163 @@
       </c>
       <c r="C74" s="15">
         <f>IF(AND(C76&gt;0,C77&gt;0,C78&gt;0,C79&gt;0,C81&gt;0,C82&gt;0,C83&gt;0,C84&gt;0,C85&gt;0,C86&gt;0,C87&gt;0),B74+1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74" s="15">
         <f t="shared" ref="D74:AP74" si="20">IF(AND(D76&gt;0,D77&gt;0,D78&gt;0,D79&gt;0,D81&gt;0,D82&gt;0,D83&gt;0,D84&gt;0,D85&gt;0,D86&gt;0,D87&gt;0),C74+1,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="N74" s="15">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="O74" s="15">
         <f t="shared" si="20"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="P74" s="15">
         <f t="shared" si="20"/>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="Q74" s="15">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="R74" s="15">
         <f t="shared" si="20"/>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="S74" s="15">
         <f t="shared" si="20"/>
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="T74" s="15">
         <f t="shared" si="20"/>
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="U74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="V74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="X74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="Y74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="Z74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AA74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AB74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AC74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AD74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AE74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AF74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AG74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AH74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AI74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AJ74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AK74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AL74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="AM74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="AN74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="AO74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="AP74" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AQ74" s="15"/>
       <c r="AR74" s="15"/>
@@ -12819,163 +12819,163 @@
       </c>
       <c r="C76" s="15">
         <f>IF(C16='Proforma Inputs'!$B74,B76+1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76" s="15">
         <f>IF(D16='Proforma Inputs'!$B74,C76+1,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E76" s="15">
         <f>IF(E16='Proforma Inputs'!$B74,D76+1,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F76" s="15">
         <f>IF(F16='Proforma Inputs'!$B74,E76+1,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G76" s="15">
         <f>IF(G16='Proforma Inputs'!$B74,F76+1,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H76" s="15">
         <f>IF(H16='Proforma Inputs'!$B74,G76+1,0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I76" s="15">
         <f>IF(I16='Proforma Inputs'!$B74,H76+1,0)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J76" s="15">
         <f>IF(J16='Proforma Inputs'!$B74,I76+1,0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K76" s="15">
         <f>IF(K16='Proforma Inputs'!$B74,J76+1,0)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L76" s="15">
         <f>IF(L16='Proforma Inputs'!$B74,K76+1,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M76" s="15">
         <f>IF(M16='Proforma Inputs'!$B74,L76+1,0)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="N76" s="15">
         <f>IF(N16='Proforma Inputs'!$B74,M76+1,0)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="O76" s="15">
         <f>IF(O16='Proforma Inputs'!$B74,N76+1,0)</f>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="P76" s="15">
         <f>IF(P16='Proforma Inputs'!$B74,O76+1,0)</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="Q76" s="15">
         <f>IF(Q16='Proforma Inputs'!$B74,P76+1,0)</f>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="R76" s="15">
         <f>IF(R16='Proforma Inputs'!$B74,Q76+1,0)</f>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="S76" s="15">
         <f>IF(S16='Proforma Inputs'!$B74,R76+1,0)</f>
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="T76" s="15">
         <f>IF(T16='Proforma Inputs'!$B74,S76+1,0)</f>
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="U76" s="15">
         <f>IF(U16='Proforma Inputs'!$B74,T76+1,0)</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="V76" s="15">
         <f>IF(V16='Proforma Inputs'!$B74,U76+1,0)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W76" s="15">
         <f>IF(W16='Proforma Inputs'!$B74,V76+1,0)</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="X76" s="15">
         <f>IF(X16='Proforma Inputs'!$B74,W76+1,0)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="Y76" s="15">
         <f>IF(Y16='Proforma Inputs'!$B74,X76+1,0)</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="Z76" s="15">
         <f>IF(Z16='Proforma Inputs'!$B74,Y76+1,0)</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AA76" s="15">
         <f>IF(AA16='Proforma Inputs'!$B74,Z76+1,0)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AB76" s="15">
         <f>IF(AB16='Proforma Inputs'!$B74,AA76+1,0)</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AC76" s="15">
         <f>IF(AC16='Proforma Inputs'!$B74,AB76+1,0)</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AD76" s="15">
         <f>IF(AD16='Proforma Inputs'!$B74,AC76+1,0)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AE76" s="15">
         <f>IF(AE16='Proforma Inputs'!$B74,AD76+1,0)</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AF76" s="15">
         <f>IF(AF16='Proforma Inputs'!$B74,AE76+1,0)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AG76" s="15">
         <f>IF(AG16='Proforma Inputs'!$B74,AF76+1,0)</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AH76" s="15">
         <f>IF(AH16='Proforma Inputs'!$B74,AG76+1,0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AI76" s="15">
         <f>IF(AI16='Proforma Inputs'!$B74,AH76+1,0)</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AJ76" s="15">
         <f>IF(AJ16='Proforma Inputs'!$B74,AI76+1,0)</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AK76" s="15">
         <f>IF(AK16='Proforma Inputs'!$B74,AJ76+1,0)</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AL76" s="15">
         <f>IF(AL16='Proforma Inputs'!$B74,AK76+1,0)</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="AM76" s="15">
         <f>IF(AM16='Proforma Inputs'!$B74,AL76+1,0)</f>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="AN76" s="15">
         <f>IF(AN16='Proforma Inputs'!$B74,AM76+1,0)</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="AO76" s="15">
         <f>IF(AO16='Proforma Inputs'!$B74,AN76+1,0)</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="AP76" s="15">
         <f>IF(AP16='Proforma Inputs'!$B74,AO76+1,0)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AQ76" s="15"/>
       <c r="AR76" s="15"/>
@@ -12993,163 +12993,163 @@
       </c>
       <c r="C77" s="15">
         <f>IF(C17='Proforma Inputs'!$B75,B77+1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77" s="15">
         <f>IF(D17='Proforma Inputs'!$B75,C77+1,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E77" s="15">
         <f>IF(E17='Proforma Inputs'!$B75,D77+1,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F77" s="15">
         <f>IF(F17='Proforma Inputs'!$B75,E77+1,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G77" s="15">
         <f>IF(G17='Proforma Inputs'!$B75,F77+1,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H77" s="15">
         <f>IF(H17='Proforma Inputs'!$B75,G77+1,0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I77" s="15">
         <f>IF(I17='Proforma Inputs'!$B75,H77+1,0)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J77" s="15">
         <f>IF(J17='Proforma Inputs'!$B75,I77+1,0)</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K77" s="15">
         <f>IF(K17='Proforma Inputs'!$B75,J77+1,0)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="L77" s="15">
         <f>IF(L17='Proforma Inputs'!$B75,K77+1,0)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="M77" s="15">
         <f>IF(M17='Proforma Inputs'!$B75,L77+1,0)</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="N77" s="15">
         <f>IF(N17='Proforma Inputs'!$B75,M77+1,0)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="O77" s="15">
         <f>IF(O17='Proforma Inputs'!$B75,N77+1,0)</f>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="P77" s="15">
         <f>IF(P17='Proforma Inputs'!$B75,O77+1,0)</f>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="Q77" s="15">
         <f>IF(Q17='Proforma Inputs'!$B75,P77+1,0)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="R77" s="15">
         <f>IF(R17='Proforma Inputs'!$B75,Q77+1,0)</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="S77" s="15">
         <f>IF(S17='Proforma Inputs'!$B75,R77+1,0)</f>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="T77" s="15">
         <f>IF(T17='Proforma Inputs'!$B75,S77+1,0)</f>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="U77" s="15">
         <f>IF(U17='Proforma Inputs'!$B75,T77+1,0)</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="V77" s="15">
         <f>IF(V17='Proforma Inputs'!$B75,U77+1,0)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W77" s="15">
         <f>IF(W17='Proforma Inputs'!$B75,V77+1,0)</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="X77" s="15">
         <f>IF(X17='Proforma Inputs'!$B75,W77+1,0)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="Y77" s="15">
         <f>IF(Y17='Proforma Inputs'!$B75,X77+1,0)</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="Z77" s="15">
         <f>IF(Z17='Proforma Inputs'!$B75,Y77+1,0)</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AA77" s="15">
         <f>IF(AA17='Proforma Inputs'!$B75,Z77+1,0)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AB77" s="15">
         <f>IF(AB17='Proforma Inputs'!$B75,AA77+1,0)</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AC77" s="15">
         <f>IF(AC17='Proforma Inputs'!$B75,AB77+1,0)</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AD77" s="15">
         <f>IF(AD17='Proforma Inputs'!$B75,AC77+1,0)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AE77" s="15">
         <f>IF(AE17='Proforma Inputs'!$B75,AD77+1,0)</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AF77" s="15">
         <f>IF(AF17='Proforma Inputs'!$B75,AE77+1,0)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AG77" s="15">
         <f>IF(AG17='Proforma Inputs'!$B75,AF77+1,0)</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AH77" s="15">
         <f>IF(AH17='Proforma Inputs'!$B75,AG77+1,0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AI77" s="15">
         <f>IF(AI17='Proforma Inputs'!$B75,AH77+1,0)</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AJ77" s="15">
         <f>IF(AJ17='Proforma Inputs'!$B75,AI77+1,0)</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AK77" s="15">
         <f>IF(AK17='Proforma Inputs'!$B75,AJ77+1,0)</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AL77" s="15">
         <f>IF(AL17='Proforma Inputs'!$B75,AK77+1,0)</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="AM77" s="15">
         <f>IF(AM17='Proforma Inputs'!$B75,AL77+1,0)</f>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="AN77" s="15">
         <f>IF(AN17='Proforma Inputs'!$B75,AM77+1,0)</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="AO77" s="15">
         <f>IF(AO17='Proforma Inputs'!$B75,AN77+1,0)</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="AP77" s="15">
         <f>IF(AP17='Proforma Inputs'!$B75,AO77+1,0)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AQ77" s="15"/>
       <c r="AR77" s="15"/>
@@ -13167,163 +13167,163 @@
       </c>
       <c r="C78" s="15">
         <f>IF(C18='Proforma Inputs'!$B76,B78+1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D78" s="15">
         <f>IF(D18='Proforma Inputs'!$B76,C78+1,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E78" s="15">
         <f>IF(E18='Proforma Inputs'!$B76,D78+1,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F78" s="15">
         <f>IF(F18='Proforma Inputs'!$B76,E78+1,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G78" s="15">
         <f>IF(G18='Proforma Inputs'!$B76,F78+1,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H78" s="15">
         <f>IF(H18='Proforma Inputs'!$B76,G78+1,0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I78" s="15">
         <f>IF(I18='Proforma Inputs'!$B76,H78+1,0)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J78" s="15">
         <f>IF(J18='Proforma Inputs'!$B76,I78+1,0)</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K78" s="15">
         <f>IF(K18='Proforma Inputs'!$B76,J78+1,0)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="L78" s="15">
         <f>IF(L18='Proforma Inputs'!$B76,K78+1,0)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="M78" s="15">
         <f>IF(M18='Proforma Inputs'!$B76,L78+1,0)</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="N78" s="15">
         <f>IF(N18='Proforma Inputs'!$B76,M78+1,0)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="O78" s="15">
         <f>IF(O18='Proforma Inputs'!$B76,N78+1,0)</f>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="P78" s="15">
         <f>IF(P18='Proforma Inputs'!$B76,O78+1,0)</f>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="Q78" s="15">
         <f>IF(Q18='Proforma Inputs'!$B76,P78+1,0)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="R78" s="15">
         <f>IF(R18='Proforma Inputs'!$B76,Q78+1,0)</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="S78" s="15">
         <f>IF(S18='Proforma Inputs'!$B76,R78+1,0)</f>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="T78" s="15">
         <f>IF(T18='Proforma Inputs'!$B76,S78+1,0)</f>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="U78" s="15">
         <f>IF(U18='Proforma Inputs'!$B76,T78+1,0)</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="V78" s="15">
         <f>IF(V18='Proforma Inputs'!$B76,U78+1,0)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W78" s="15">
         <f>IF(W18='Proforma Inputs'!$B76,V78+1,0)</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="X78" s="15">
         <f>IF(X18='Proforma Inputs'!$B76,W78+1,0)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="Y78" s="15">
         <f>IF(Y18='Proforma Inputs'!$B76,X78+1,0)</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="Z78" s="15">
         <f>IF(Z18='Proforma Inputs'!$B76,Y78+1,0)</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AA78" s="15">
         <f>IF(AA18='Proforma Inputs'!$B76,Z78+1,0)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AB78" s="15">
         <f>IF(AB18='Proforma Inputs'!$B76,AA78+1,0)</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AC78" s="15">
         <f>IF(AC18='Proforma Inputs'!$B76,AB78+1,0)</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AD78" s="15">
         <f>IF(AD18='Proforma Inputs'!$B76,AC78+1,0)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AE78" s="15">
         <f>IF(AE18='Proforma Inputs'!$B76,AD78+1,0)</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AF78" s="15">
         <f>IF(AF18='Proforma Inputs'!$B76,AE78+1,0)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AG78" s="15">
         <f>IF(AG18='Proforma Inputs'!$B76,AF78+1,0)</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AH78" s="15">
         <f>IF(AH18='Proforma Inputs'!$B76,AG78+1,0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AI78" s="15">
         <f>IF(AI18='Proforma Inputs'!$B76,AH78+1,0)</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AJ78" s="15">
         <f>IF(AJ18='Proforma Inputs'!$B76,AI78+1,0)</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AK78" s="15">
         <f>IF(AK18='Proforma Inputs'!$B76,AJ78+1,0)</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AL78" s="15">
         <f>IF(AL18='Proforma Inputs'!$B76,AK78+1,0)</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="AM78" s="15">
         <f>IF(AM18='Proforma Inputs'!$B76,AL78+1,0)</f>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="AN78" s="15">
         <f>IF(AN18='Proforma Inputs'!$B76,AM78+1,0)</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="AO78" s="15">
         <f>IF(AO18='Proforma Inputs'!$B76,AN78+1,0)</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="AP78" s="15">
         <f>IF(AP18='Proforma Inputs'!$B76,AO78+1,0)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AQ78" s="15"/>
       <c r="AR78" s="15"/>
@@ -13341,163 +13341,163 @@
       </c>
       <c r="C79" s="15">
         <f>IF(C19='Proforma Inputs'!$B77,B79+1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D79" s="15">
         <f>IF(D19='Proforma Inputs'!$B77,C79+1,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E79" s="15">
         <f>IF(E19='Proforma Inputs'!$B77,D79+1,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F79" s="15">
         <f>IF(F19='Proforma Inputs'!$B77,E79+1,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G79" s="15">
         <f>IF(G19='Proforma Inputs'!$B77,F79+1,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H79" s="15">
         <f>IF(H19='Proforma Inputs'!$B77,G79+1,0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I79" s="15">
         <f>IF(I19='Proforma Inputs'!$B77,H79+1,0)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J79" s="15">
         <f>IF(J19='Proforma Inputs'!$B77,I79+1,0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K79" s="15">
         <f>IF(K19='Proforma Inputs'!$B77,J79+1,0)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L79" s="15">
         <f>IF(L19='Proforma Inputs'!$B77,K79+1,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M79" s="15">
         <f>IF(M19='Proforma Inputs'!$B77,L79+1,0)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="N79" s="15">
         <f>IF(N19='Proforma Inputs'!$B77,M79+1,0)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="O79" s="15">
         <f>IF(O19='Proforma Inputs'!$B77,N79+1,0)</f>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="P79" s="15">
         <f>IF(P19='Proforma Inputs'!$B77,O79+1,0)</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="Q79" s="15">
         <f>IF(Q19='Proforma Inputs'!$B77,P79+1,0)</f>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="R79" s="15">
         <f>IF(R19='Proforma Inputs'!$B77,Q79+1,0)</f>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="S79" s="15">
         <f>IF(S19='Proforma Inputs'!$B77,R79+1,0)</f>
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="T79" s="15">
         <f>IF(T19='Proforma Inputs'!$B77,S79+1,0)</f>
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="U79" s="15">
         <f>IF(U19='Proforma Inputs'!$B77,T79+1,0)</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="V79" s="15">
         <f>IF(V19='Proforma Inputs'!$B77,U79+1,0)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W79" s="15">
         <f>IF(W19='Proforma Inputs'!$B77,V79+1,0)</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="X79" s="15">
         <f>IF(X19='Proforma Inputs'!$B77,W79+1,0)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="Y79" s="15">
         <f>IF(Y19='Proforma Inputs'!$B77,X79+1,0)</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="Z79" s="15">
         <f>IF(Z19='Proforma Inputs'!$B77,Y79+1,0)</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AA79" s="15">
         <f>IF(AA19='Proforma Inputs'!$B77,Z79+1,0)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AB79" s="15">
         <f>IF(AB19='Proforma Inputs'!$B77,AA79+1,0)</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AC79" s="15">
         <f>IF(AC19='Proforma Inputs'!$B77,AB79+1,0)</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AD79" s="15">
         <f>IF(AD19='Proforma Inputs'!$B77,AC79+1,0)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AE79" s="15">
         <f>IF(AE19='Proforma Inputs'!$B77,AD79+1,0)</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AF79" s="15">
         <f>IF(AF19='Proforma Inputs'!$B77,AE79+1,0)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AG79" s="15">
         <f>IF(AG19='Proforma Inputs'!$B77,AF79+1,0)</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AH79" s="15">
         <f>IF(AH19='Proforma Inputs'!$B77,AG79+1,0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AI79" s="15">
         <f>IF(AI19='Proforma Inputs'!$B77,AH79+1,0)</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AJ79" s="15">
         <f>IF(AJ19='Proforma Inputs'!$B77,AI79+1,0)</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AK79" s="15">
         <f>IF(AK19='Proforma Inputs'!$B77,AJ79+1,0)</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AL79" s="15">
         <f>IF(AL19='Proforma Inputs'!$B77,AK79+1,0)</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="AM79" s="15">
         <f>IF(AM19='Proforma Inputs'!$B77,AL79+1,0)</f>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="AN79" s="15">
         <f>IF(AN19='Proforma Inputs'!$B77,AM79+1,0)</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="AO79" s="15">
         <f>IF(AO19='Proforma Inputs'!$B77,AN79+1,0)</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="AP79" s="15">
         <f>IF(AP19='Proforma Inputs'!$B77,AO79+1,0)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AQ79" s="15"/>
       <c r="AR79" s="15"/>
@@ -13567,163 +13567,163 @@
       </c>
       <c r="C81" s="15">
         <f>IF(C21='Proforma Inputs'!$B92,B81+1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D81" s="15">
         <f>IF(D21='Proforma Inputs'!$B92,C81+1,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E81" s="15">
         <f>IF(E21='Proforma Inputs'!$B92,D81+1,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F81" s="15">
         <f>IF(F21='Proforma Inputs'!$B92,E81+1,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G81" s="15">
         <f>IF(G21='Proforma Inputs'!$B92,F81+1,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H81" s="15">
         <f>IF(H21='Proforma Inputs'!$B92,G81+1,0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I81" s="15">
         <f>IF(I21='Proforma Inputs'!$B92,H81+1,0)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J81" s="15">
         <f>IF(J21='Proforma Inputs'!$B92,I81+1,0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K81" s="15">
         <f>IF(K21='Proforma Inputs'!$B92,J81+1,0)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L81" s="15">
         <f>IF(L21='Proforma Inputs'!$B92,K81+1,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M81" s="15">
         <f>IF(M21='Proforma Inputs'!$B92,L81+1,0)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="N81" s="15">
         <f>IF(N21='Proforma Inputs'!$B92,M81+1,0)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="O81" s="15">
         <f>IF(O21='Proforma Inputs'!$B92,N81+1,0)</f>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="P81" s="15">
         <f>IF(P21='Proforma Inputs'!$B92,O81+1,0)</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="Q81" s="15">
         <f>IF(Q21='Proforma Inputs'!$B92,P81+1,0)</f>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="R81" s="15">
         <f>IF(R21='Proforma Inputs'!$B92,Q81+1,0)</f>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="S81" s="15">
         <f>IF(S21='Proforma Inputs'!$B92,R81+1,0)</f>
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="T81" s="15">
         <f>IF(T21='Proforma Inputs'!$B92,S81+1,0)</f>
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="U81" s="15">
         <f>IF(U21='Proforma Inputs'!$B92,T81+1,0)</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="V81" s="15">
         <f>IF(V21='Proforma Inputs'!$B92,U81+1,0)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W81" s="15">
         <f>IF(W21='Proforma Inputs'!$B92,V81+1,0)</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="X81" s="15">
         <f>IF(X21='Proforma Inputs'!$B92,W81+1,0)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="Y81" s="15">
         <f>IF(Y21='Proforma Inputs'!$B92,X81+1,0)</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="Z81" s="15">
         <f>IF(Z21='Proforma Inputs'!$B92,Y81+1,0)</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AA81" s="15">
         <f>IF(AA21='Proforma Inputs'!$B92,Z81+1,0)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AB81" s="15">
         <f>IF(AB21='Proforma Inputs'!$B92,AA81+1,0)</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AC81" s="15">
         <f>IF(AC21='Proforma Inputs'!$B92,AB81+1,0)</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AD81" s="15">
         <f>IF(AD21='Proforma Inputs'!$B92,AC81+1,0)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AE81" s="15">
         <f>IF(AE21='Proforma Inputs'!$B92,AD81+1,0)</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AF81" s="15">
         <f>IF(AF21='Proforma Inputs'!$B92,AE81+1,0)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AG81" s="15">
         <f>IF(AG21='Proforma Inputs'!$B92,AF81+1,0)</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AH81" s="15">
         <f>IF(AH21='Proforma Inputs'!$B92,AG81+1,0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AI81" s="15">
         <f>IF(AI21='Proforma Inputs'!$B92,AH81+1,0)</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AJ81" s="15">
         <f>IF(AJ21='Proforma Inputs'!$B92,AI81+1,0)</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AK81" s="15">
         <f>IF(AK21='Proforma Inputs'!$B92,AJ81+1,0)</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AL81" s="15">
         <f>IF(AL21='Proforma Inputs'!$B92,AK81+1,0)</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="AM81" s="15">
         <f>IF(AM21='Proforma Inputs'!$B92,AL81+1,0)</f>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="AN81" s="15">
         <f>IF(AN21='Proforma Inputs'!$B92,AM81+1,0)</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="AO81" s="15">
         <f>IF(AO21='Proforma Inputs'!$B92,AN81+1,0)</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="AP81" s="15">
         <f>IF(AP21='Proforma Inputs'!$B92,AO81+1,0)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AQ81" s="15"/>
       <c r="AR81" s="15"/>
@@ -14801,7 +14801,7 @@
       </c>
       <c r="G88" s="15">
         <f>IF(OR(SUM($B$88:F88)=1,SUM(G59:G67)&gt;0),0,IF(OR(G74&gt;'Proforma Inputs'!$B$8,G3&gt;='Proforma Inputs'!$B$6*'Proforma Inputs'!$B$4+('Proforma Inputs'!$B$44-1)),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H88" s="15">
         <f>IF(OR(SUM($B$88:G88)=1,SUM(H59:H67)&gt;0),0,IF(OR(H74&gt;'Proforma Inputs'!$B$8,H3&gt;='Proforma Inputs'!$B$6*'Proforma Inputs'!$B$4+('Proforma Inputs'!$B$44-1)),1,0))</f>
@@ -14853,7 +14853,7 @@
       </c>
       <c r="T88" s="15">
         <f>IF(OR(SUM($B$88:S88)=1,SUM(T59:T67)&gt;0),0,IF(OR(T74&gt;'Proforma Inputs'!$B$8,T3&gt;='Proforma Inputs'!$B$6*'Proforma Inputs'!$B$4+('Proforma Inputs'!$B$44-1)),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U88" s="15">
         <f>IF(OR(SUM($B$88:T88)=1,SUM(U59:U67)&gt;0),0,IF(OR(U74&gt;'Proforma Inputs'!$B$8,U3&gt;='Proforma Inputs'!$B$6*'Proforma Inputs'!$B$4+('Proforma Inputs'!$B$44-1)),1,0))</f>
@@ -14979,55 +14979,55 @@
       </c>
       <c r="H89" s="15">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I89" s="15">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J89" s="15">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K89" s="15">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L89" s="15">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M89" s="15">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N89" s="15">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O89" s="15">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P89" s="15">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q89" s="15">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R89" s="15">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S89" s="15">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T89" s="15">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U89" s="15">
         <f t="shared" si="21"/>
@@ -15149,59 +15149,59 @@
       </c>
       <c r="G90" s="5">
         <f t="shared" si="22"/>
-        <v>141145.83333333334</v>
+        <v>-8500</v>
       </c>
       <c r="H90" s="5">
         <f t="shared" si="22"/>
-        <v>707291.66666666663</v>
+        <v>0</v>
       </c>
       <c r="I90" s="5">
         <f t="shared" si="22"/>
-        <v>1273437.5</v>
+        <v>0</v>
       </c>
       <c r="J90" s="5">
         <f t="shared" si="22"/>
-        <v>1839583.3333333333</v>
+        <v>0</v>
       </c>
       <c r="K90" s="5">
         <f t="shared" si="22"/>
-        <v>2309375</v>
+        <v>0</v>
       </c>
       <c r="L90" s="5">
         <f t="shared" si="22"/>
-        <v>2779166.6666666665</v>
+        <v>0</v>
       </c>
       <c r="M90" s="5">
         <f t="shared" si="22"/>
-        <v>3248958.3333333335</v>
+        <v>0</v>
       </c>
       <c r="N90" s="5">
         <f t="shared" si="22"/>
-        <v>3718750</v>
+        <v>0</v>
       </c>
       <c r="O90" s="5">
         <f t="shared" si="22"/>
-        <v>3718750</v>
+        <v>0</v>
       </c>
       <c r="P90" s="5">
         <f t="shared" si="22"/>
-        <v>3718750</v>
+        <v>0</v>
       </c>
       <c r="Q90" s="5">
         <f t="shared" si="22"/>
-        <v>3718750</v>
+        <v>0</v>
       </c>
       <c r="R90" s="5">
         <f t="shared" si="22"/>
-        <v>3718750</v>
+        <v>0</v>
       </c>
       <c r="S90" s="5">
         <f t="shared" si="22"/>
-        <v>3718750</v>
+        <v>0</v>
       </c>
       <c r="T90" s="5">
         <f t="shared" si="22"/>
-        <v>3718750</v>
+        <v>0</v>
       </c>
       <c r="U90" s="5">
         <f t="shared" si="22"/>
@@ -15323,59 +15323,59 @@
       </c>
       <c r="G91" s="5">
         <f>G90/'Proforma Inputs'!$B$14</f>
-        <v>2016369.0476190476</v>
+        <v>-121428.57142857142</v>
       </c>
       <c r="H91" s="5">
         <f>H90/'Proforma Inputs'!$B$14</f>
-        <v>10104166.666666666</v>
+        <v>0</v>
       </c>
       <c r="I91" s="5">
         <f>I90/'Proforma Inputs'!$B$14</f>
-        <v>18191964.285714284</v>
+        <v>0</v>
       </c>
       <c r="J91" s="5">
         <f>J90/'Proforma Inputs'!$B$14</f>
-        <v>26279761.904761903</v>
+        <v>0</v>
       </c>
       <c r="K91" s="5">
         <f>K90/'Proforma Inputs'!$B$14</f>
-        <v>32991071.428571425</v>
+        <v>0</v>
       </c>
       <c r="L91" s="5">
         <f>L90/'Proforma Inputs'!$B$14</f>
-        <v>39702380.952380948</v>
+        <v>0</v>
       </c>
       <c r="M91" s="5">
         <f>M90/'Proforma Inputs'!$B$14</f>
-        <v>46413690.476190478</v>
+        <v>0</v>
       </c>
       <c r="N91" s="5">
         <f>N90/'Proforma Inputs'!$B$14</f>
-        <v>53124999.999999993</v>
+        <v>0</v>
       </c>
       <c r="O91" s="5">
         <f>O90/'Proforma Inputs'!$B$14</f>
-        <v>53124999.999999993</v>
+        <v>0</v>
       </c>
       <c r="P91" s="5">
         <f>P90/'Proforma Inputs'!$B$14</f>
-        <v>53124999.999999993</v>
+        <v>0</v>
       </c>
       <c r="Q91" s="5">
         <f>Q90/'Proforma Inputs'!$B$14</f>
-        <v>53124999.999999993</v>
+        <v>0</v>
       </c>
       <c r="R91" s="5">
         <f>R90/'Proforma Inputs'!$B$14</f>
-        <v>53124999.999999993</v>
+        <v>0</v>
       </c>
       <c r="S91" s="5">
         <f>S90/'Proforma Inputs'!$B$14</f>
-        <v>53124999.999999993</v>
+        <v>0</v>
       </c>
       <c r="T91" s="5">
         <f>T90/'Proforma Inputs'!$B$14</f>
-        <v>53124999.999999993</v>
+        <v>0</v>
       </c>
       <c r="U91" s="5">
         <f>U90/'Proforma Inputs'!$B$14</f>
@@ -15567,8 +15567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -15660,7 +15660,6 @@
         <v>36</v>
       </c>
       <c r="B12" s="51">
-        <f>0.085</f>
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="D12" t="s">
@@ -15942,7 +15941,8 @@
         <v>216</v>
       </c>
       <c r="B40" s="17">
-        <v>30000000</v>
+        <f>SUM('Cost Model'!D63:D102)</f>
+        <v>0</v>
       </c>
       <c r="C40" t="s">
         <v>152</v>
@@ -15956,7 +15956,7 @@
         <v>169</v>
       </c>
       <c r="B41" s="48">
-        <v>5000000</v>
+        <v>100000</v>
       </c>
       <c r="C41" t="s">
         <v>152</v>
@@ -16012,7 +16012,8 @@
         <v>219</v>
       </c>
       <c r="B48" s="5">
-        <v>2000000</v>
+        <f>'Revenue Model'!B21*'Revenue Model'!B141</f>
+        <v>0</v>
       </c>
       <c r="C48" t="s">
         <v>152</v>
@@ -16026,7 +16027,8 @@
         <v>30</v>
       </c>
       <c r="B49" s="5">
-        <v>3000000</v>
+        <f>'Revenue Model'!B22*'Revenue Model'!B142</f>
+        <v>0</v>
       </c>
       <c r="C49" t="s">
         <v>152</v>
@@ -16040,7 +16042,8 @@
         <v>31</v>
       </c>
       <c r="B50" s="5">
-        <v>4000000</v>
+        <f>'Revenue Model'!B23*'Revenue Model'!B143</f>
+        <v>0</v>
       </c>
       <c r="C50" t="s">
         <v>152</v>
@@ -16054,7 +16057,8 @@
         <v>32</v>
       </c>
       <c r="B51" s="5">
-        <v>5000000</v>
+        <f>'Revenue Model'!B24*'Revenue Model'!B144</f>
+        <v>0</v>
       </c>
       <c r="C51" t="s">
         <v>152</v>
@@ -16074,7 +16078,8 @@
         <v>219</v>
       </c>
       <c r="B53" s="32">
-        <v>250000</v>
+        <f>B48*0.2+1</f>
+        <v>1</v>
       </c>
       <c r="C53" t="s">
         <v>204</v>
@@ -16087,8 +16092,9 @@
       <c r="A54" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B54" s="17">
-        <v>300000</v>
+      <c r="B54" s="32">
+        <f t="shared" ref="B54:B56" si="0">B49*0.2+1</f>
+        <v>1</v>
       </c>
       <c r="C54" t="s">
         <v>204</v>
@@ -16102,7 +16108,8 @@
         <v>31</v>
       </c>
       <c r="B55" s="32">
-        <v>350000</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="C55" t="s">
         <v>204</v>
@@ -16116,7 +16123,8 @@
         <v>32</v>
       </c>
       <c r="B56" s="32">
-        <v>400000</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="C56" t="s">
         <v>204</v>
@@ -16212,8 +16220,8 @@
         <v>219</v>
       </c>
       <c r="B65" s="32">
-        <f>B60/(('Revenue Model'!B53+'Revenue Model'!B58+'Revenue Model'!B146)/IF('Revenue Model'!B48=0,1,'Revenue Model'!B48))</f>
-        <v>0</v>
+        <f>B60*0.2+1</f>
+        <v>1</v>
       </c>
       <c r="C65" t="s">
         <v>204</v>
@@ -16227,8 +16235,8 @@
         <v>30</v>
       </c>
       <c r="B66" s="32">
-        <f>B61/(('Revenue Model'!B54+'Revenue Model'!B59+'Revenue Model'!B147)/IF('Revenue Model'!B49=0,1,'Revenue Model'!B49))</f>
-        <v>0</v>
+        <f t="shared" ref="B66:B68" si="1">B61*0.2+1</f>
+        <v>1</v>
       </c>
       <c r="C66" t="s">
         <v>204</v>
@@ -16242,8 +16250,8 @@
         <v>31</v>
       </c>
       <c r="B67" s="32">
-        <f>B62/(('Revenue Model'!B55+'Revenue Model'!B60+'Revenue Model'!B148)/IF('Revenue Model'!B50=0,1,'Revenue Model'!B50))</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="C67" t="s">
         <v>204</v>
@@ -16257,8 +16265,8 @@
         <v>32</v>
       </c>
       <c r="B68" s="32">
-        <f>B63/(('Revenue Model'!B56+'Revenue Model'!B61+'Revenue Model'!B149)/IF('Revenue Model'!B51=0,1,'Revenue Model'!B51))</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="C68" t="s">
         <v>204</v>
@@ -16282,7 +16290,7 @@
         <v>170</v>
       </c>
       <c r="B71" s="19">
-        <v>75000</v>
+        <v>7500</v>
       </c>
       <c r="C71" t="s">
         <v>28</v>
@@ -16296,7 +16304,7 @@
         <v>125</v>
       </c>
       <c r="B72" s="19">
-        <v>75000</v>
+        <v>7500</v>
       </c>
       <c r="C72" t="s">
         <v>28</v>
@@ -16321,7 +16329,8 @@
         <v>219</v>
       </c>
       <c r="B74" s="5">
-        <v>100000</v>
+        <f>'Revenue Model'!B70*'Revenue Model'!B151/$B$4</f>
+        <v>0</v>
       </c>
       <c r="C74" t="s">
         <v>204</v>
@@ -16335,7 +16344,8 @@
         <v>30</v>
       </c>
       <c r="B75" s="5">
-        <v>200000</v>
+        <f>'Revenue Model'!B71*'Revenue Model'!B152/$B$4</f>
+        <v>0</v>
       </c>
       <c r="C75" t="s">
         <v>204</v>
@@ -16349,7 +16359,8 @@
         <v>31</v>
       </c>
       <c r="B76" s="5">
-        <v>300000</v>
+        <f>'Revenue Model'!B72*'Revenue Model'!B153/$B$4</f>
+        <v>0</v>
       </c>
       <c r="C76" t="s">
         <v>204</v>
@@ -16363,7 +16374,8 @@
         <v>32</v>
       </c>
       <c r="B77" s="5">
-        <v>400000</v>
+        <f>'Revenue Model'!B73*'Revenue Model'!B154/$B$4</f>
+        <v>0</v>
       </c>
       <c r="C77" t="s">
         <v>204</v>
@@ -16444,7 +16456,7 @@
         <v>219</v>
       </c>
       <c r="B84" s="41">
-        <v>8.3333333333333329E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="D84" t="s">
         <v>121</v>
@@ -16455,8 +16467,7 @@
         <v>30</v>
       </c>
       <c r="B85" s="41">
-        <f>0.5/12</f>
-        <v>4.1666666666666664E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="D85" t="s">
         <v>121</v>
@@ -16467,8 +16478,7 @@
         <v>31</v>
       </c>
       <c r="B86" s="41">
-        <f>0.25/12</f>
-        <v>2.0833333333333332E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="D86" t="s">
         <v>121</v>
@@ -16479,8 +16489,7 @@
         <v>32</v>
       </c>
       <c r="B87" s="41">
-        <f>1/12</f>
-        <v>8.3333333333333329E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="D87" t="s">
         <v>121</v>
@@ -16502,7 +16511,8 @@
         <v>1</v>
       </c>
       <c r="B92" s="17">
-        <v>4000000</v>
+        <f>'Revenue Model'!B97*'Revenue Model'!B156/$B$4</f>
+        <v>0</v>
       </c>
       <c r="C92" t="s">
         <v>204</v>
@@ -16611,7 +16621,8 @@
         <v>1</v>
       </c>
       <c r="B100" s="37">
-        <v>8</v>
+        <f>('Revenue Model'!B156+'Revenue Model'!B121+'Revenue Model'!B113)/IF('Revenue Model'!B105=0,1,'Revenue Model'!B105)</f>
+        <v>6</v>
       </c>
       <c r="C100" t="s">
         <v>214</v>
@@ -16720,8 +16731,8 @@
         <v>1</v>
       </c>
       <c r="B108" s="1">
-        <f>0.6/12</f>
-        <v>4.9999999999999996E-2</v>
+        <f>'Revenue Model'!B113/'Revenue Model'!B129</f>
+        <v>0.05</v>
       </c>
       <c r="C108" t="s">
         <v>126</v>
@@ -16831,8 +16842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D162"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A124" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -19540,8 +19551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V113"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="112" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="112" workbookViewId="0">
+      <selection activeCell="J79" sqref="J79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -21759,7 +21770,7 @@
         <v>0</v>
       </c>
       <c r="J78" s="83">
-        <f>C78*(J88-C6)</f>
+        <f>MAX(C78*(J88-C6),0)</f>
         <v>0</v>
       </c>
       <c r="K78" s="134">

</xml_diff>